<commit_message>
Add a row to sheets in template
7.1.0 -> 7.1.1
</commit_message>
<xml_diff>
--- a/Template for Generator R7.xlsx
+++ b/Template for Generator R7.xlsx
@@ -138,7 +138,7 @@
     <t>Version:</t>
   </si>
   <si>
-    <t>7.1.0</t>
+    <t>7.1.1</t>
   </si>
   <si>
     <t>Rundown ID</t>
@@ -1914,7 +1914,7 @@
       </c>
       <c r="J3" s="15">
         <f>rand()</f>
-        <v>0.670360269</v>
+        <v>0.902000032</v>
       </c>
     </row>
     <row r="4">
@@ -5153,25 +5153,37 @@
       <c r="J22" s="11"/>
       <c r="K22" s="11"/>
     </row>
+    <row r="23">
+      <c r="A23" s="25"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="22"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="C3:C22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="C3:C23">
       <formula1>"GoToElevator,GoToExitGeo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a ZonePlacementDatas and then add it to the ChainedObjectiveData." sqref="D3:D22">
-      <formula1>'ExpeditionInTier Lists'!F$3:F22</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a ZonePlacementDatas and then add it to the ChainedObjectiveData." sqref="D3:D23">
+      <formula1>'ExpeditionInTier Lists'!F$3:F23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="H3:H22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="H3:H23">
       <formula1>"Zone_0,Zone_1,Zone_2,Zone_3,Zone_4,Zone_5,Zone_6,Zone_7,Zone_8,Zone_9,Zone_10,Zone_11,Zone_12,Zone_13,Zone_14,Zone_15,Zone_16,Zone_17,Zone_18,Zone_19,Zone_20"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 4,294,967,295" sqref="B3:B22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between 0 and 4,294,967,295" sqref="B3:B23">
       <formula1>0.0</formula1>
       <formula2>4.294967295E9</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="G3:G22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="G3:G23">
       <formula1>"Reality,Dimension_1,Dimension_2,Dimension_3,Dimension_4,Dimension_5,Dimension_6,Dimension_7,Dimension_8,Dimension_9,Dimension_10,Dimension_11,Dimension_12,Dimension_13,Dimension_14,Dimension_15,Dimension_16,Dimension_17,Dimension_18,Dimension_19,Dimension"&amp;"_20,MAX_COUNT,ARENA_DIMENSION"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="I3:K22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="I3:K23">
       <formula1>-3.402823E38</formula1>
       <formula2>3.402823E38</formula2>
     </dataValidation>
@@ -8082,58 +8094,182 @@
       <c r="CO22" s="11"/>
       <c r="CP22" s="16"/>
     </row>
+    <row r="23">
+      <c r="A23" s="12"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="16"/>
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
+      <c r="AE23" s="16"/>
+      <c r="AF23" s="28"/>
+      <c r="AG23" s="14"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="16"/>
+      <c r="AJ23" s="20"/>
+      <c r="AK23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN23" s="12"/>
+      <c r="AO23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="12"/>
+      <c r="AR23" s="28"/>
+      <c r="AS23" s="9"/>
+      <c r="AT23" s="9"/>
+      <c r="AU23" s="19"/>
+      <c r="AV23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW23" s="20"/>
+      <c r="AX23" s="20"/>
+      <c r="AY23" s="9"/>
+      <c r="AZ23" s="16"/>
+      <c r="BA23" s="16"/>
+      <c r="BB23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BC23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BD23" s="9"/>
+      <c r="BE23" s="21"/>
+      <c r="BF23" s="21"/>
+      <c r="BG23" s="16"/>
+      <c r="BH23" s="9"/>
+      <c r="BI23" s="9"/>
+      <c r="BJ23" s="9"/>
+      <c r="BK23" s="9"/>
+      <c r="BL23" s="28"/>
+      <c r="BM23" s="28"/>
+      <c r="BN23" s="28"/>
+      <c r="BO23" s="28"/>
+      <c r="BP23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BQ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BR23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BS23" s="20"/>
+      <c r="BT23" s="20"/>
+      <c r="BU23" s="16"/>
+      <c r="BV23" s="16"/>
+      <c r="BW23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BX23" s="16"/>
+      <c r="BY23" s="16"/>
+      <c r="BZ23" s="11"/>
+      <c r="CA23" s="11"/>
+      <c r="CB23" s="11"/>
+      <c r="CC23" s="11"/>
+      <c r="CD23" s="11"/>
+      <c r="CE23" s="11"/>
+      <c r="CF23" s="11"/>
+      <c r="CG23" s="11"/>
+      <c r="CH23" s="11"/>
+      <c r="CI23" s="11"/>
+      <c r="CJ23" s="11"/>
+      <c r="CK23" s="11"/>
+      <c r="CL23" s="11"/>
+      <c r="CM23" s="11"/>
+      <c r="CN23" s="11"/>
+      <c r="CO23" s="11"/>
+      <c r="CP23" s="16"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="U3:U22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="U3:U23">
       <formula1>"LowMidHigh,OnlyLow,OnlyHigh,OnlyMid,LowMid,MidHigh,LowHigh,Ascending,Descending,Unchanged"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AJ3:AJ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AJ3:AJ23">
       <formula1>"Single x1,Single x1_No_close_HUD,Single red x1 No alarm,Checkpoint,Single Small x1,Single Bigger x1,Cluster Small x1,Small Cluster x3 - No Alarm Stealth,Small Cluster x3 - No Alarm Stealth_Far,Small Cluster x2 - No Alarm Stealth,Single D10 req all x1,Team"&amp;" req all x1,single x1 R6A1 Narrative lock,single x1 R6C1 Narrative lock 1,single x1 R6C1 Narrative lock 2,single x1 R6C1 Narrative lock 3,single x1 R6C1 Narrative lock 4,Single x1 - No alarm,HSU_Scan,ExpeditionExit_Scan,ExpeditionExit_Scan_Team,Single x1 "&amp;"- Alarm,Single x1 - Alarm Birther,Single Far x1 - Alarm,Single Far x1 - Alarm Shooters,Single x1 - Alarm Bullrush,Single x1 - Alarm Trickle 2-5,Single x1 - Alarm Trickle 4-6 Bullrush Bigs,Single x2 - Alarm Diminished,Single x2 - Alarm Even More Diminished"&amp;",Single x2 - Alarm Tutorial,Single x2 - Alarm,Single bigger x2 Far - Alarm Halved,Single Bigger x1 Alarm,Single Bigger Separated x2 Alarm,Single Bundled x3 - Alarm,Single x4 - Alarm,Single bigger x3 Far - Alarm,Single bigger x3 Far - Alarm Halved,Single b"&amp;"igger x3 Far - Alarm Halved Bullrush,Single bigger x5  - Alarm,Single Big x6 - Alarm with flyers,Single bigger x4  - Alarm Flyers,Single bigger x5  - Alarm Shadows,Single x1 Moving 58 static points - Alarm,Single x1 Moving 22 static points - Alarm,Single "&amp;"x1 Moving 11 static points - Alarm,Single x1 Moving 3 random points - Alarm Bullrush mix,Single sustained x5 - Alarm Bullrush Mix,Single bigger x1 - Alarm Trickle 2-5,Mixed Separated x3 - Alarm,Mixed Sustained x5 - Alarm Bullrush Mix,Mixed x6 alarm,Mixed "&amp;"x3 - Alarm Diminished,Mixed x4 - Alarm Diminished,Mixed x4 - Alarm Diminished_1AreaSpawn,Mixed x3 - Alarm,Mixed Big x3 - Alarm Reduced Bullrush Mix,Mixed Bundled x3 - Alarm,Mixed x4 - Alarm Halved Bullrush,Mixed x4 Separated - Alarm Shooters,Mixed x4 Sepa"&amp;"rated - Alarm,Mixed x4 - Alarm,Mixed x4 - Alarm Hybrids,Mixed Far x4 - Alarm,Mixed x4 - Alarm Reduced Few Shadows,Mixed x5 - Alarm,Mixed x5 - Alarm Hybrids,Mixed x5 - Alarm_Far,Mixed x5 - Alarm Flyers Spawn Points,Mixed Far Bundled No Req All x5 - Alarm R"&amp;"educed Shadows,Mixed x5 Bundled - Alarm,Mixed Far x5 - Alarm Reduced Bullrush Mix,Mixed Far Separated x5 - Alarm,Mixed Big Cluster Separated x5 - Alarm Hybrids,Mixed x5 - Alarm Diminished,Mixed x5 - Alarm Diminished_Shadows,Mixed x5 - Alarm Diminished_Bul"&amp;"lrush,Mixed Separated x5 - Alarm,Mixed Separated x6 - No alarm,Mixed Separated x5 - Alarm Hybrids,Mixed Separated Far x5 - Alarm Hybrids,Mixed  x6 - Alarm Reduced Bullrush,Mixed Far x6 - Alarm Reduced Bullrush Mix,Mixed Far x6 - Alarm,Mixed Bigs Separated"&amp;" x6 - Alarm Hybrids Modified,Mixed Far Separated x7 - Alarm,Mixed x6 - Alarm Shadows Mixed,Mixed Bigs Separated x4 - Alarm Hybrids,Mixed Far Bundled x3 - Alarm Shadows,Mixed Bundled x3 - Alarm  Reduced Shadows,Mixed Bundled x5 - Alarm Shadows,Mixed Separa"&amp;"ted Far x10 - Alarm,Mixed Separated Far x10 - Alarm_BullRush,Mixed Separated Far x10 - Alarm_Shadows,Mixed Irregular x5 - Alarm Shadows,Mixed Irregular x6 - Alarm Shadows,Mixed Irregular x7 - Alarm Hybrids Modified,Mixed Irregular x5 - Alarm Third Bigs,Mi"&amp;"xed Irregular x7 - Alarm Third Bigs,Mixed Irregular x6 - Alarm Diminished,Mixed Irregular x3 - Alarm Reduced Bullrush Mix,Mixed Irregular x4 - Alarm Reduced Bullrush Mix,Mixed Irregular x4 - Alarm Reduced Bullrush,OLD Chained bioscan mix,Single x1 - Error"&amp;" Alarm Trickle 3-52,Single x1 - Error Alarm Apex Wave From Elevator,Single x1 - Error Alarm Apex Wave From Elevator No Flyers,Single x1 - Error Alarm wave Mainframe,Single x1 - Error Alarm Trickle 4-6 Bullrush Bigs,Single x1 - Error Alarm Trickle 2-45 Bul"&amp;"lrush Bigs,Single x1 - Error Alarm Trickle 3-45 Bullrush Bigs,Single x1 - Error Alarm Trickle 3-30 Hybrids Modified,Single x1 - Error Alarm Trickle 6-30 Shadows,Single x1 - Error Alarm Trickle 4-20 Bullrush,Single x1 - Error Alarm Trickle 5-45 Bullrush,Si"&amp;"ngle x1 - Error Alarm Trickle 4-40 Bigs,Single x1 - Error Alarm Trickle 6-160 Bullrush,Single x1 - Error Alarm Trickle 2-15,Single small x1 - Error Alarm Bullrush Trickle 6-30 Build-up,Single x1 - Error Alarm Big Shadows Trickle 4-60,Single x1 - Error Ala"&amp;"rm Shadows Trickle 8-10 Spawnpoint,Single x1 - Error Alarm Trickle 6-20 From Elevator,Single x1 - Error Alarm Trickle 6-15 Sp-Flyer,Mixed Irregular x4 - Error Alarm Reduced Bullrush Mix,Single Sustained Defend Far x1 - Alarm Diminished,Single Sustained De"&amp;"fend Far x1 - Alarm Increased Hybrids,Single Sustained Defend x1 - Alarm Increased,Single Sustained Defend x1 - Alarm Increased BioscanPoint,Single Sustained Defend x1 - Alarm Increased Further,Single Sustained Defend x1 - Alarm Hybrids Modified,Single Su"&amp;"stained Defend Far x1 - Alarm Hybrids Modifier,Single Sustained Far x3 - Alarm,Single Sustained Far x3 - Alarm Bullrush Miniboss,Single Sustained x4 Far - Alarm,Single Sustained Far x6 - Alarm Increased,Single Sustained x6 - Alarm,Single Sustained Far Bun"&amp;"dled x5 - Alarm Hybrids Modified,Cluster Sustained Far x1 - Alarm,Mixed Sustained Far Separated x3 - Alarm Reduced Bullrush Mix,Cluster x3 - Alarm Diminished Bullrush,Mixed Far Sustained x5 - Alarm Reduced Shadows and Flyers,Mixed Sustained Separated x9 -"&amp;" Diminished Alarm Hybrids,Single Sustained Defend Far x1 - Alarm Surge,Single Sustained Defend MegaHuge x1 - Alarm No Wave,Single Sustained Zone Scan - Alarm 3 sides,Single Sustained Zone Scan - Alarm 3 sides v2,Single Sustained Zone Scan - Alarm Bullrush"&amp;",Single Sustained Zone Scan - Alarm R7D1,Single Sustained Zone Scan - PouncerWaves,Single Sustained Zone Scan No Graphics- Alarm,Single Sustained Defend Huge x1 Alarm Tanks Late,Single Sustained Defend Huge x1 Alarm Birther Late,Cluster x2 - Alarm,Cluster"&amp;" x3 - Alarm,Mixed Cluster big x4 - Alarm,Cluster x3 - Alarm Easier,Cluster x4 - Alarm,Cluster x4 - Alarm - Pouncer,Cluster x5 - Alarm Reduced Bullrush,Cluster x6 - Alarm Reduced Bullrush,Cluster x7 - Alarm Reduced Bullrush,Cluster x7 - Alarm,Cluster x6 - "&amp;"Alarm,Cluster x5 - Alarm,Cluster x5 - Alarm Far,Cluster x4 - Alarm Far,Cluster x4 - Alarm Pretty Far,Cluster x8 - Alarm,Small Cluster x2 - Alarm Shooters,Small Cluster x2 - Alarm Reduced Bullrush,Small Cluster x2 - Alarm,Small Cluster Separated x3 - Alarm"&amp;" Bullrush,Small Cluster Bundled x3 - Alarm,Small Cluster x3 - Alarm Shooters,Small Cluster Separated x3 - Alarm Hybrids Modified,Small Cluster Separated x4 - Alarm,Small Cluster Separated x4 - Alarm Far Diminished,Small Cluster Separated x4 - Alarm Hybrid"&amp;"s,Small Cluster Separated x4 - Alarm Bullrush,Small Cluster Bundled x3 - Alarm_duplicate,Single Far Separated x4 - Alarm Surge,Single Far Separated More x3 - Alarm Surge Hybrids,Mixed Far Separated x3 - Alarm Surge Hybrids,Single Far Separated x4 - Alarm "&amp;"Surge Hybrids,Single Sustained Far Separated x4 - Alarm Surge Hybrids,SecurityScan_Bulkhead_Select_Layer_Main,SecurityScan_Bulkhead_Select_Layer_Secondary,SecurityScan_Bulkhead_Select_Layer_Third"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="J3:J22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="J3:J23">
       <formula1>"DigSite,Refinery,Storage,DataCenter,Lab,All,Floodways,Mining_Reactor,Plug_SubComplex_Transition,Tech_Reactor,Tech_Portal,Gardens,Mining_Portal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AN3:AN22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AN3:AN23">
       <formula1>"Security,Apex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="T3:T22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="T3:T23">
       <formula1>"BlueToOrange_1,Tutorial_StealthSpotlight,OrangeToBlue_1,RedToCyan_1,HeavyRedToCyan_1,WashedOutRed_1,OrangeToYellow_1,PurpleToBlue_1,Monochrome_Orange,Monochrome_Orange_Flickering,Monochrome_Blue,Monochrome_Blue_Flickering,Monochrome_Cyan,Monochrome_iceblu"&amp;"e,Monochrome_Red,RedToWhite_1,RedToWhite_1_Flickering,RedToYellow_1,Monochrome_Yellow,Monochrome_YellowToGreen,Monochrome_Green,Monochrome_Red_Copy,Monochrome_Red_R7D1,BlueToGreen_1,BlueToPink_1,PurpleToOrange_1,CyanBrownToYellow_1,OrangeToBrown_1,RustyRe"&amp;"dToBrown_1,CyanToPurple_1,Pitch_black_1,Totally_black,DarkGreenToRed_1,DarkGreenToOrange_1,OrangeToBluishGrey,DarkBlue_1,DarkGreyToOrange,DarkGrey_1,DarkBlueToPurple_1,PurpleToRed_1,PurpleToPink_1,CyanToYellow_1,YellowToCyan_1,AlmostWhite_1,ColdWhite_all_"&amp;"on_1,CyanToBlue_1,YellowToOrange_1,GreenToRed_1,BlueToRed_1,Reactor_blue_to_red_all_on_1,Reactor_green_all_on_1,Reactor_blue_to_White_all_on_1,White_To_Blue_all_on_1,TGA_1_INTRO_CyanToBlue,TGA_2_COCOONS_CyanToBlue,TGA_3_ARTIFACT_YellowToCyan,TGA_4_IMMORTA"&amp;"L_GreenToRed,TGA_5_HSU_BlueToRed,BlueGreen-&gt;Brown,DarktealToYellow,PeachToGreen,PurpleToBrown,OrangeToBlue,New,monochrome,New_Copy_Copy_1,camo_green,HSU_Prep_R7D1,Mainframe_R7D2"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="S3:S22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="S3:S23">
       <formula1>"Random,Collapsed,Expansional,Directional_Forward,Directional_Backward,Directional_Right,Directional_Left,Directional_Random"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="BL3:BO22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="BL3:BO23">
       <formula1>"None_0,Pair_2,Few_5,Some_10,SomeMore_15,Many_20,Alot_30,Tons_50"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="BT3:BT22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="BT3:BT23">
       <formula1>"BaselineTest,Defoggers_2,PowerCell_1,PowerCell_Defogger,PowerCell_2,PowerCell_3,Defoggers_1,Small_HSUs_10,Datasphere,MWP_1,Sedatives_1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AR3:AR22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AR3:AR23">
       <formula1>"None,SessionSeed,BuildSeed,StaticSeed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="BS3:BS22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="BS3:BS23">
       <formula1>"Baseline_c1_r3,Baseline_a2_r3,ExplorationFog,OnlyFogReps,ExplorationDark,Darkness,Baseline_small,CombatFog_medium,CombatMelee_Storage,Combat_MineFocus_Storage,CombatMelee_Storage_lessMelee,CombatMelee_Storage_Medium,CombatFog_BiggerMedium,Small_foam,Small"&amp;"_Foam,Small_explosives_Tripmine,Small_fog,Tiny_fog,Small_C-foam,Abundant C-foam,Baseline,Baseline_Fog,Baseline_c2_r6,Baseline_lots_in_containers,Baseline_Tech,Baseline_small_Tech,Baseline_small_Tech_R4,Baseline_small_Tech_R4_fog,ExplorationFog_Tech,Explor"&amp;"ationDark_Tech,ExplorationDark_Tech_R4,CombatFog_medium_Tech,Small_fog_Tech,ExplorationFog_Tech_v02,Freps_IIX_glows_Tech,Foam_Tech,Stealth_Tech,Explosives_Tech,Syringes_disinfect_Tech,PickUp_MemoryStick_Interactable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="A3:A22 O3:O22 AQ3:AQ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="A3:A23 O3:O23 AQ3:AQ23">
       <formula1>"Zone_0,Zone_1,Zone_2,Zone_3,Zone_4,Zone_5,Zone_6,Zone_7,Zone_8,Zone_9,Zone_10,Zone_11,Zone_12,Zone_13,Zone_14,Zone_15,Zone_16,Zone_17,Zone_18,Zone_19,Zone_20"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="R3:R22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="R3:R23">
       <formula1>"Towards_Random,Towards_Forward,Towards_Backward,Towards_Right,Towards_Left"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AW3:AX22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AW3:AX23">
       <formula1>"Hibernate Easy Large Melee,Hibernate Easy Mix,Hibernate Easy Small Mix A,Hibernate Easy Small Mix B,Hibernate Easy Tiny Mix A,Hibernate Easy Tiny Mix B,Hibernate Easy Tiny Melee,Hibernate Medium Mix A,Hibernate Medium Mix B,Hibernate Medium Small Mix A,Hi"&amp;"bernate Medium Small Mix B,Hibernate Medium Tiny Mix A,Hibernate Medium Tiny Mix B,Hibernate Medium Tiny Melee,Hibernate Hard Large Mix Scout,Hibernate Hard Large Mix,Hibernate Hard Mix Scout,Hibernate Hard Small Mix A,Hibernate Hard Small Mix Scout,Hiber"&amp;"nate Hard Small Mix B,Hibernate Hard Large Scout,Hibernate Biss Large Melee Shadows,Hibernate Biss Melee Shadows,Hibernate Biss Small Melee Shadows,Hibernate Biss Tiny Melee Shadows,Hibernate Buss Melee Big Shadows,Hibernate Buss Small Melee Big Shadows,P"&amp;"ure Sneak Easy,Pure Sneak Medium,Pure Sneak Hard Birther Align_1,Pure Sneak Biss Hybrids,Pure Sneak Buss Large BirtherChild,Pure Sneak Buss BirtherChild,Pure Sneak Buss Small BirtherChild,Hibernate Miniboss Minibos Birther Align_0,Hibernate Miniboss Megab"&amp;"oss Tank Align_0,Hibernate Boss Boss BirtherBoss Align_1,Hibernate Pure Sneak Miniboss BirtherBoss Align_1,Pure Sneak Boss Boss Squidward Align_0,Pure Sneak Megaboss Tank,Pure Detect Easy Scout,Pure Detect Medium Scout,Pure Detect Hard Scout,Pure Detect B"&amp;"oss Shadow Scout,Pure Detect MiniBoss Bullrush Scout,Detect Lurker Bullrush Striker,Detect Lurker Small Bullrush Striker,Detect Lurker Medium Bullrush Striker,Detect Lurker Hard Small Bullrush Bigs,Detect Lurker Hard Large Bullrush Bigs,Detect Lurker Mini"&amp;"boss ???,detect_hard_scout,Bullrush,Hunter Easy Infront strikers shooters,Hunter Medium Inback strikers shooters,Hunter Boss Birther,Hunter Boss Birther Only One,Hunter Boss Tank,Hunter Bigs,Hunter Miniboss BirtherBoss,Hunter Easy Inback Strikers+Shooters"&amp;"+Hybrids,Hunter Easy Inback Strikers+Shooters+Hybrids V2,Hunter Medium Inback Strikers+Shooters+Hybrids,Hunter Easy Bullrush,Hunter Easy Large Bullrush,Hunter Medium Biss Melee Shadows,Birther Boss Children,Birther Children,PatrolTest,Squid Boss Children,"&amp;"Hunter Biss Pouncer"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -4294967296 and 4294967295" sqref="B3:B22 D3:I22 AH3:AH22 AS3:AT22 AY3:AY22 BD3:BD22 BH3:BK22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -4294967296 and 4294967295" sqref="B3:B23 D3:I23 AH3:AH23 AS3:AT23 AY3:AY23 BD3:BD23 BH3:BK23">
       <formula1>-4.294967296E9</formula1>
       <formula2>4.294967295E9</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="P3:P22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="P3:P23">
       <formula1>"From_Random,From_Start,From_AverageCenter,From_Furthest,From_BetweenStartAndFurthest,From_IndexWeight"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AF3:AF22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AF3:AF23">
       <formula1>"None,Keycard_SecurityBox,PowerGenerator_And_PowerCell,Locked_No_Key"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="M3:N22 Q3:Q22 V3:V22 BE3:BF22 BZ3:CO22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="M3:N23 Q3:Q23 V3:V23 BE3:BF23 BZ3:CO23">
       <formula1>-3.402823E38</formula1>
       <formula2>3.402823E38</formula2>
     </dataValidation>
@@ -8155,9 +8291,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75" outlineLevelCol="3"/>
   <cols>
-    <col collapsed="1" min="3" max="3" width="12.63"/>
+    <col collapsed="1" customWidth="1" min="3" max="3" width="12.63"/>
     <col hidden="1" min="4" max="11" width="12.63" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="13" max="13" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="13" max="13" width="16.63"/>
     <col customWidth="1" hidden="1" min="14" max="14" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="15" max="15" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="16" max="17" width="12.63" outlineLevel="1"/>
@@ -8181,7 +8317,7 @@
     <col customWidth="1" hidden="1" min="46" max="46" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="47" max="47" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="48" max="48" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="50" max="50" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="50" max="50" width="19.0"/>
     <col customWidth="1" hidden="1" min="51" max="51" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="52" max="52" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="53" max="54" width="12.63" outlineLevel="1"/>
@@ -8205,7 +8341,7 @@
     <col customWidth="1" hidden="1" min="83" max="83" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="84" max="84" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="85" max="85" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="87" max="87" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="87" max="87" width="17.0"/>
     <col customWidth="1" hidden="1" min="88" max="88" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="89" max="89" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="90" max="91" width="12.63" outlineLevel="1"/>
@@ -8229,7 +8365,7 @@
     <col customWidth="1" hidden="1" min="120" max="120" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="121" max="121" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="122" max="122" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="124" max="124" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="124" max="124" width="16.0"/>
     <col customWidth="1" hidden="1" min="125" max="125" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="126" max="126" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="127" max="128" width="12.63" outlineLevel="1"/>
@@ -8253,7 +8389,7 @@
     <col customWidth="1" hidden="1" min="157" max="157" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="158" max="158" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="159" max="159" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="161" max="161" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="161" max="161" width="19.25"/>
     <col customWidth="1" hidden="1" min="162" max="162" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="163" max="163" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="164" max="165" width="12.63" outlineLevel="1"/>
@@ -8277,7 +8413,7 @@
     <col customWidth="1" hidden="1" min="194" max="194" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="195" max="195" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="196" max="196" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="198" max="198" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="198" max="198" width="19.75"/>
     <col customWidth="1" hidden="1" min="199" max="199" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="200" max="200" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="201" max="202" width="12.63" outlineLevel="1"/>
@@ -8301,7 +8437,7 @@
     <col customWidth="1" hidden="1" min="231" max="231" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="232" max="232" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="233" max="233" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="235" max="235" width="16.25"/>
+    <col collapsed="1" customWidth="1" min="235" max="235" width="16.5"/>
     <col customWidth="1" hidden="1" min="236" max="236" width="24.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="237" max="237" width="13.13" outlineLevel="1"/>
     <col hidden="1" min="238" max="239" width="12.63" outlineLevel="1"/>
@@ -8350,7 +8486,7 @@
     <col customWidth="1" hidden="1" min="306" max="306" width="29.38" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="307" max="307" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="308" max="308" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="310" max="310" width="20.25"/>
+    <col collapsed="1" customWidth="1" min="310" max="310" width="20.63"/>
     <col hidden="1" min="311" max="311" width="12.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="312" max="312" width="15.75" outlineLevel="1"/>
     <col hidden="1" min="313" max="316" width="12.63" outlineLevel="1"/>
@@ -8379,7 +8515,7 @@
     <col customWidth="1" hidden="1" min="352" max="352" width="19.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="353" max="353" width="19.5" outlineLevel="1"/>
     <col customWidth="1" min="354" max="354" width="18.13"/>
-    <col collapsed="1" customWidth="1" min="355" max="355" width="18.13"/>
+    <col collapsed="1" customWidth="1" min="355" max="355" width="25.13"/>
     <col customWidth="1" hidden="1" min="356" max="356" width="51.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="357" max="357" width="19.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="358" max="359" width="18.13" outlineLevel="1"/>
@@ -8407,51 +8543,51 @@
     <col customWidth="1" hidden="1" min="393" max="393" width="29.38" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="394" max="394" width="19.63" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="395" max="395" width="19.5" outlineLevel="2"/>
-    <col collapsed="1" customWidth="1" min="397" max="397" width="17.88"/>
+    <col collapsed="1" customWidth="1" min="397" max="397" width="18.75"/>
     <col customWidth="1" hidden="1" min="398" max="398" width="25.13" outlineLevel="1"/>
     <col hidden="1" min="399" max="401" width="12.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="402" max="402" width="14.75" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="404" max="404" width="20.88"/>
+    <col collapsed="1" customWidth="1" min="404" max="404" width="21.63"/>
     <col customWidth="1" hidden="1" min="405" max="405" width="23.13" outlineLevel="1"/>
-    <col collapsed="1" min="407" max="407" width="12.63"/>
+    <col collapsed="1" customWidth="1" min="407" max="407" width="23.5"/>
     <col customWidth="1" hidden="1" min="408" max="408" width="32.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="409" max="409" width="19.5" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="411" max="411" width="15.75"/>
-    <col hidden="1" min="412" max="417" width="12.63" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="418" max="418" width="14.5" outlineLevel="1"/>
-    <col hidden="1" min="419" max="419" width="12.63" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="420" max="420" width="16.63" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="421" max="421" width="13.5" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="422" max="422" width="24.25" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="423" max="423" width="14.5" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="424" max="424" width="13.38" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="425" max="425" width="16.5" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="426" max="426" width="13.38" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="427" max="427" width="15.38" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="428" max="428" width="16.13" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="429" max="429" width="16.88" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="430" max="430" width="18.88" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="431" max="431" width="24.0" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="432" max="432" width="19.75" outlineLevel="1"/>
-    <col hidden="1" min="433" max="433" width="12.63" outlineLevel="1"/>
-    <col collapsed="1" hidden="1" min="434" max="434" width="12.63" outlineLevel="1"/>
+    <col customWidth="1" min="411" max="411" width="16.0"/>
+    <col min="412" max="417" width="12.63" outlineLevel="1"/>
+    <col customWidth="1" min="418" max="418" width="14.5" outlineLevel="1"/>
+    <col min="419" max="419" width="12.63" outlineLevel="1"/>
+    <col customWidth="1" min="420" max="420" width="16.63" outlineLevel="1"/>
+    <col customWidth="1" min="421" max="421" width="13.5" outlineLevel="1"/>
+    <col customWidth="1" min="422" max="422" width="24.25" outlineLevel="1"/>
+    <col customWidth="1" min="423" max="423" width="14.5" outlineLevel="1"/>
+    <col customWidth="1" min="424" max="424" width="13.38" outlineLevel="1"/>
+    <col customWidth="1" min="425" max="425" width="16.5" outlineLevel="1"/>
+    <col customWidth="1" min="426" max="426" width="13.38" outlineLevel="1"/>
+    <col customWidth="1" min="427" max="427" width="15.38" outlineLevel="1"/>
+    <col customWidth="1" min="428" max="428" width="16.13" outlineLevel="1"/>
+    <col customWidth="1" min="429" max="429" width="16.88" outlineLevel="1"/>
+    <col customWidth="1" min="430" max="430" width="18.88" outlineLevel="1"/>
+    <col customWidth="1" min="431" max="431" width="24.0" outlineLevel="1"/>
+    <col customWidth="1" min="432" max="432" width="19.75" outlineLevel="1"/>
+    <col min="433" max="433" width="12.63" outlineLevel="1"/>
+    <col collapsed="1" min="434" max="434" width="12.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="435" max="437" width="25.13" outlineLevel="2"/>
     <col hidden="1" min="438" max="438" width="12.63" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="439" max="439" width="19.75" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="440" max="440" width="27.25" outlineLevel="2"/>
-    <col hidden="1" min="441" max="441" width="12.63" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" hidden="1" min="442" max="442" width="14.5" outlineLevel="1"/>
-    <col customWidth="1" hidden="1" min="443" max="444" width="25.13" outlineLevel="2"/>
-    <col customWidth="1" hidden="1" min="445" max="445" width="18.0" outlineLevel="2"/>
-    <col customWidth="1" hidden="1" min="446" max="446" width="19.38" outlineLevel="2"/>
-    <col customWidth="1" hidden="1" min="447" max="447" width="18.75" outlineLevel="2"/>
-    <col customWidth="1" hidden="1" min="448" max="448" width="12.63" outlineLevel="2"/>
-    <col collapsed="1" customWidth="1" hidden="1" min="449" max="449" width="15.5" outlineLevel="2"/>
+    <col min="441" max="441" width="12.63" outlineLevel="1"/>
+    <col customWidth="1" min="442" max="442" width="14.5" outlineLevel="1"/>
+    <col customWidth="1" min="443" max="444" width="25.13" outlineLevel="2"/>
+    <col customWidth="1" min="445" max="445" width="18.0" outlineLevel="2"/>
+    <col customWidth="1" min="446" max="446" width="19.38" outlineLevel="2"/>
+    <col customWidth="1" min="447" max="447" width="18.75" outlineLevel="2"/>
+    <col customWidth="1" min="448" max="448" width="12.63" outlineLevel="2"/>
+    <col collapsed="1" customWidth="1" min="449" max="449" width="15.5" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="450" max="450" width="18.88" outlineLevel="3"/>
     <col customWidth="1" hidden="1" min="451" max="451" width="25.13" outlineLevel="3"/>
     <col customWidth="1" hidden="1" min="452" max="452" width="12.63" outlineLevel="3"/>
-    <col customWidth="1" hidden="1" min="453" max="453" width="12.63" outlineLevel="2"/>
-    <col collapsed="1" customWidth="1" hidden="1" min="454" max="454" width="19.38" outlineLevel="2"/>
+    <col customWidth="1" min="453" max="453" width="12.63" outlineLevel="2"/>
+    <col collapsed="1" customWidth="1" min="454" max="454" width="19.38" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="455" max="455" width="24.5" outlineLevel="3"/>
     <col customWidth="1" hidden="1" min="456" max="456" width="13.13" outlineLevel="3"/>
     <col hidden="1" min="457" max="458" width="12.63" outlineLevel="3"/>
@@ -8475,21 +8611,21 @@
     <col customWidth="1" hidden="1" min="487" max="487" width="29.38" outlineLevel="3"/>
     <col customWidth="1" hidden="1" min="488" max="488" width="19.63" outlineLevel="3"/>
     <col customWidth="1" hidden="1" min="489" max="489" width="19.5" outlineLevel="3"/>
-    <col hidden="1" min="490" max="490" width="12.63" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" hidden="1" min="491" max="491" width="19.75" outlineLevel="1"/>
+    <col min="490" max="490" width="12.63" outlineLevel="1"/>
+    <col collapsed="1" customWidth="1" min="491" max="491" width="19.75" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="492" max="492" width="13.88" outlineLevel="2"/>
     <col hidden="1" min="493" max="493" width="12.63" outlineLevel="2"/>
     <col customWidth="1" hidden="1" min="494" max="494" width="13.88" outlineLevel="2"/>
     <col hidden="1" min="495" max="498" width="12.63" outlineLevel="2"/>
-    <col collapsed="1" customWidth="1" min="500" max="500" width="21.13"/>
+    <col collapsed="1" customWidth="1" min="500" max="500" width="21.88"/>
     <col hidden="1" min="501" max="503" width="12.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="504" max="504" width="13.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="505" max="505" width="15.25" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="507" max="507" width="23.25"/>
+    <col collapsed="1" customWidth="1" min="507" max="507" width="23.5"/>
     <col hidden="1" min="508" max="510" width="12.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="511" max="511" width="13.5" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="512" max="512" width="15.25" outlineLevel="1"/>
-    <col collapsed="1" customWidth="1" min="514" max="514" width="21.13"/>
+    <col collapsed="1" customWidth="1" min="514" max="514" width="21.88"/>
     <col hidden="1" min="515" max="515" width="12.63" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="516" max="516" width="28.75" outlineLevel="1"/>
     <col customWidth="1" hidden="1" min="517" max="517" width="15.88" outlineLevel="1"/>
@@ -8678,7 +8814,7 @@
       <c r="JE1" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="JL1" s="16" t="s">
+      <c r="JL1" s="19" t="s">
         <v>227</v>
       </c>
       <c r="JM1" s="16"/>
@@ -23099,107 +23235,739 @@
       <c r="SZ22" s="13"/>
       <c r="TA22" s="9"/>
     </row>
+    <row r="23">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="22"/>
+      <c r="J23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="32"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="11"/>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="33"/>
+      <c r="AA23" s="33"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="32"/>
+      <c r="AD23" s="33"/>
+      <c r="AE23" s="20"/>
+      <c r="AF23" s="20"/>
+      <c r="AG23" s="11"/>
+      <c r="AH23" s="20"/>
+      <c r="AI23" s="20"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM23" s="33"/>
+      <c r="AN23" s="20"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="11"/>
+      <c r="AQ23" s="11"/>
+      <c r="AR23" s="9"/>
+      <c r="AS23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT23" s="28"/>
+      <c r="AU23" s="28"/>
+      <c r="AV23" s="7"/>
+      <c r="AX23" s="12"/>
+      <c r="AY23" s="28"/>
+      <c r="AZ23" s="9"/>
+      <c r="BA23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BB23" s="12"/>
+      <c r="BC23" s="20"/>
+      <c r="BD23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BE23" s="12"/>
+      <c r="BF23" s="12"/>
+      <c r="BG23" s="12"/>
+      <c r="BH23" s="11"/>
+      <c r="BI23" s="11"/>
+      <c r="BJ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BK23" s="33"/>
+      <c r="BL23" s="33"/>
+      <c r="BM23" s="33"/>
+      <c r="BN23" s="32"/>
+      <c r="BO23" s="33"/>
+      <c r="BP23" s="20"/>
+      <c r="BQ23" s="20"/>
+      <c r="BR23" s="11"/>
+      <c r="BS23" s="20"/>
+      <c r="BT23" s="20"/>
+      <c r="BU23" s="9"/>
+      <c r="BV23" s="11"/>
+      <c r="BW23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BX23" s="33"/>
+      <c r="BY23" s="20"/>
+      <c r="BZ23" s="11"/>
+      <c r="CA23" s="11"/>
+      <c r="CB23" s="11"/>
+      <c r="CC23" s="9"/>
+      <c r="CD23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CE23" s="28"/>
+      <c r="CF23" s="28"/>
+      <c r="CG23" s="7"/>
+      <c r="CI23" s="12"/>
+      <c r="CJ23" s="28"/>
+      <c r="CK23" s="9"/>
+      <c r="CL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CM23" s="12"/>
+      <c r="CN23" s="20"/>
+      <c r="CO23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CP23" s="12"/>
+      <c r="CQ23" s="12"/>
+      <c r="CR23" s="12"/>
+      <c r="CS23" s="11"/>
+      <c r="CT23" s="11"/>
+      <c r="CU23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CV23" s="33"/>
+      <c r="CW23" s="33"/>
+      <c r="CX23" s="33"/>
+      <c r="CY23" s="32"/>
+      <c r="CZ23" s="33"/>
+      <c r="DA23" s="20"/>
+      <c r="DB23" s="20"/>
+      <c r="DC23" s="11"/>
+      <c r="DD23" s="20"/>
+      <c r="DE23" s="20"/>
+      <c r="DF23" s="9"/>
+      <c r="DG23" s="11"/>
+      <c r="DH23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="DI23" s="33"/>
+      <c r="DJ23" s="20"/>
+      <c r="DK23" s="11"/>
+      <c r="DL23" s="11"/>
+      <c r="DM23" s="11"/>
+      <c r="DN23" s="9"/>
+      <c r="DO23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="DP23" s="28"/>
+      <c r="DQ23" s="28"/>
+      <c r="DR23" s="7"/>
+      <c r="DS23" s="19"/>
+      <c r="DT23" s="12"/>
+      <c r="DU23" s="28"/>
+      <c r="DV23" s="9"/>
+      <c r="DW23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="DX23" s="12"/>
+      <c r="DY23" s="20"/>
+      <c r="DZ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="EA23" s="12"/>
+      <c r="EB23" s="12"/>
+      <c r="EC23" s="12"/>
+      <c r="ED23" s="11"/>
+      <c r="EE23" s="11"/>
+      <c r="EF23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="EG23" s="33"/>
+      <c r="EH23" s="33"/>
+      <c r="EI23" s="33"/>
+      <c r="EJ23" s="32"/>
+      <c r="EK23" s="33"/>
+      <c r="EL23" s="20"/>
+      <c r="EM23" s="20"/>
+      <c r="EN23" s="11"/>
+      <c r="EO23" s="20"/>
+      <c r="EP23" s="20"/>
+      <c r="EQ23" s="9"/>
+      <c r="ER23" s="11"/>
+      <c r="ES23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="ET23" s="33"/>
+      <c r="EU23" s="20"/>
+      <c r="EV23" s="11"/>
+      <c r="EW23" s="11"/>
+      <c r="EX23" s="11"/>
+      <c r="EY23" s="9"/>
+      <c r="EZ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="FA23" s="28"/>
+      <c r="FB23" s="28"/>
+      <c r="FC23" s="7"/>
+      <c r="FE23" s="12"/>
+      <c r="FF23" s="28"/>
+      <c r="FG23" s="9"/>
+      <c r="FH23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="FI23" s="12"/>
+      <c r="FJ23" s="20"/>
+      <c r="FK23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="FL23" s="12"/>
+      <c r="FM23" s="12"/>
+      <c r="FN23" s="12"/>
+      <c r="FO23" s="11"/>
+      <c r="FP23" s="11"/>
+      <c r="FQ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="FR23" s="33"/>
+      <c r="FS23" s="33"/>
+      <c r="FT23" s="33"/>
+      <c r="FU23" s="32"/>
+      <c r="FV23" s="33"/>
+      <c r="FW23" s="20"/>
+      <c r="FX23" s="20"/>
+      <c r="FY23" s="11"/>
+      <c r="FZ23" s="20"/>
+      <c r="GA23" s="20"/>
+      <c r="GB23" s="9"/>
+      <c r="GC23" s="11"/>
+      <c r="GD23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="GE23" s="33"/>
+      <c r="GF23" s="20"/>
+      <c r="GG23" s="11"/>
+      <c r="GH23" s="11"/>
+      <c r="GI23" s="11"/>
+      <c r="GJ23" s="9"/>
+      <c r="GK23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="GL23" s="28"/>
+      <c r="GM23" s="28"/>
+      <c r="GN23" s="7"/>
+      <c r="GP23" s="12"/>
+      <c r="GQ23" s="28"/>
+      <c r="GR23" s="9"/>
+      <c r="GS23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="GT23" s="12"/>
+      <c r="GU23" s="20"/>
+      <c r="GV23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="GW23" s="12"/>
+      <c r="GX23" s="12"/>
+      <c r="GY23" s="12"/>
+      <c r="GZ23" s="11"/>
+      <c r="HA23" s="11"/>
+      <c r="HB23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="HC23" s="33"/>
+      <c r="HD23" s="33"/>
+      <c r="HE23" s="33"/>
+      <c r="HF23" s="32"/>
+      <c r="HG23" s="33"/>
+      <c r="HH23" s="20"/>
+      <c r="HI23" s="20"/>
+      <c r="HJ23" s="11"/>
+      <c r="HK23" s="20"/>
+      <c r="HL23" s="20"/>
+      <c r="HM23" s="9"/>
+      <c r="HN23" s="11"/>
+      <c r="HO23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="HP23" s="33"/>
+      <c r="HQ23" s="20"/>
+      <c r="HR23" s="11"/>
+      <c r="HS23" s="11"/>
+      <c r="HT23" s="11"/>
+      <c r="HU23" s="9"/>
+      <c r="HV23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="HW23" s="28"/>
+      <c r="HX23" s="28"/>
+      <c r="HY23" s="7"/>
+      <c r="IA23" s="12"/>
+      <c r="IB23" s="28"/>
+      <c r="IC23" s="9"/>
+      <c r="ID23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="IE23" s="12"/>
+      <c r="IF23" s="20"/>
+      <c r="IG23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="IH23" s="12"/>
+      <c r="II23" s="12"/>
+      <c r="IJ23" s="12"/>
+      <c r="IK23" s="11"/>
+      <c r="IL23" s="11"/>
+      <c r="IM23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="IN23" s="33"/>
+      <c r="IO23" s="33"/>
+      <c r="IP23" s="33"/>
+      <c r="IQ23" s="32"/>
+      <c r="IR23" s="33"/>
+      <c r="IS23" s="20"/>
+      <c r="IT23" s="20"/>
+      <c r="IU23" s="11"/>
+      <c r="IV23" s="20"/>
+      <c r="IW23" s="20"/>
+      <c r="IX23" s="9"/>
+      <c r="IY23" s="11"/>
+      <c r="IZ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="JA23" s="33"/>
+      <c r="JB23" s="20"/>
+      <c r="JC23" s="11"/>
+      <c r="JD23" s="11"/>
+      <c r="JE23" s="11"/>
+      <c r="JF23" s="9"/>
+      <c r="JG23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="JH23" s="28"/>
+      <c r="JI23" s="28"/>
+      <c r="JJ23" s="7"/>
+      <c r="JL23" s="12"/>
+      <c r="JM23" s="7"/>
+      <c r="JN23" s="28"/>
+      <c r="JO23" s="9"/>
+      <c r="JP23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="JQ23" s="12"/>
+      <c r="JR23" s="20"/>
+      <c r="JS23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="JT23" s="12"/>
+      <c r="JU23" s="12"/>
+      <c r="JV23" s="12"/>
+      <c r="JW23" s="11"/>
+      <c r="JX23" s="11"/>
+      <c r="JY23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="JZ23" s="33"/>
+      <c r="KA23" s="33"/>
+      <c r="KB23" s="33"/>
+      <c r="KC23" s="32"/>
+      <c r="KD23" s="33"/>
+      <c r="KE23" s="20"/>
+      <c r="KF23" s="20"/>
+      <c r="KG23" s="11"/>
+      <c r="KH23" s="20"/>
+      <c r="KI23" s="20"/>
+      <c r="KJ23" s="9"/>
+      <c r="KK23" s="11"/>
+      <c r="KL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="KM23" s="33"/>
+      <c r="KN23" s="20"/>
+      <c r="KO23" s="11"/>
+      <c r="KP23" s="11"/>
+      <c r="KQ23" s="11"/>
+      <c r="KR23" s="9"/>
+      <c r="KS23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="KT23" s="28"/>
+      <c r="KU23" s="28"/>
+      <c r="KV23" s="7"/>
+      <c r="KX23" s="12"/>
+      <c r="KY23" s="16"/>
+      <c r="KZ23" s="12"/>
+      <c r="LA23" s="12"/>
+      <c r="LB23" s="11"/>
+      <c r="LC23" s="11"/>
+      <c r="LD23" s="11"/>
+      <c r="LF23" s="12"/>
+      <c r="LG23" s="28"/>
+      <c r="LH23" s="9"/>
+      <c r="LI23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="LJ23" s="12"/>
+      <c r="LK23" s="20"/>
+      <c r="LL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="LM23" s="12"/>
+      <c r="LN23" s="12"/>
+      <c r="LO23" s="12"/>
+      <c r="LP23" s="11"/>
+      <c r="LQ23" s="11"/>
+      <c r="LR23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="LS23" s="33"/>
+      <c r="LT23" s="33"/>
+      <c r="LU23" s="33"/>
+      <c r="LV23" s="32"/>
+      <c r="LW23" s="33"/>
+      <c r="LX23" s="20"/>
+      <c r="LY23" s="20"/>
+      <c r="LZ23" s="11"/>
+      <c r="MA23" s="20"/>
+      <c r="MB23" s="20"/>
+      <c r="MC23" s="9"/>
+      <c r="MD23" s="11"/>
+      <c r="ME23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="MF23" s="33"/>
+      <c r="MG23" s="20"/>
+      <c r="MH23" s="11"/>
+      <c r="MI23" s="11"/>
+      <c r="MJ23" s="11"/>
+      <c r="MK23" s="9"/>
+      <c r="ML23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="MM23" s="28"/>
+      <c r="MN23" s="28"/>
+      <c r="MO23" s="7"/>
+      <c r="MQ23" s="12"/>
+      <c r="MR23" s="20"/>
+      <c r="MS23" s="7"/>
+      <c r="MT23" s="22"/>
+      <c r="MV23" s="25"/>
+      <c r="MW23" s="28"/>
+      <c r="MX23" s="9"/>
+      <c r="MY23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="MZ23" s="12"/>
+      <c r="NA23" s="20"/>
+      <c r="NB23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="NC23" s="12"/>
+      <c r="ND23" s="12"/>
+      <c r="NE23" s="12"/>
+      <c r="NF23" s="11"/>
+      <c r="NG23" s="11"/>
+      <c r="NH23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="NI23" s="33"/>
+      <c r="NJ23" s="33"/>
+      <c r="NK23" s="33"/>
+      <c r="NL23" s="32"/>
+      <c r="NM23" s="33"/>
+      <c r="NN23" s="20"/>
+      <c r="NO23" s="20"/>
+      <c r="NP23" s="11"/>
+      <c r="NQ23" s="20"/>
+      <c r="NR23" s="20"/>
+      <c r="NS23" s="9"/>
+      <c r="NT23" s="11"/>
+      <c r="NU23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="NV23" s="33"/>
+      <c r="NW23" s="20"/>
+      <c r="NX23" s="11"/>
+      <c r="NY23" s="11"/>
+      <c r="NZ23" s="11"/>
+      <c r="OA23" s="9"/>
+      <c r="OB23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="OC23" s="28"/>
+      <c r="OD23" s="28"/>
+      <c r="OE23" s="7"/>
+      <c r="OG23" s="12"/>
+      <c r="OH23" s="16"/>
+      <c r="OI23" s="12"/>
+      <c r="OJ23" s="12"/>
+      <c r="OK23" s="12"/>
+      <c r="OL23" s="11"/>
+      <c r="ON23" s="12"/>
+      <c r="OO23" s="20"/>
+      <c r="OQ23" s="12"/>
+      <c r="OR23" s="20"/>
+      <c r="OS23" s="22"/>
+      <c r="OU23" s="12"/>
+      <c r="OV23" s="11"/>
+      <c r="OW23" s="11"/>
+      <c r="OX23" s="11"/>
+      <c r="OY23" s="9"/>
+      <c r="OZ23" s="9"/>
+      <c r="PA23" s="22"/>
+      <c r="PB23" s="22"/>
+      <c r="PC23" s="12"/>
+      <c r="PD23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="PE23" s="14"/>
+      <c r="PF23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="PG23" s="10"/>
+      <c r="PH23" s="10"/>
+      <c r="PI23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="PJ23" s="7"/>
+      <c r="PK23" s="7"/>
+      <c r="PL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="PM23" s="9"/>
+      <c r="PN23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="PO23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="PP23" s="22"/>
+      <c r="PR23" s="22"/>
+      <c r="PS23" s="22"/>
+      <c r="PT23" s="14"/>
+      <c r="PU23" s="12"/>
+      <c r="PV23" s="10"/>
+      <c r="PW23" s="9"/>
+      <c r="PX23" s="10"/>
+      <c r="PY23" s="16"/>
+      <c r="PZ23" s="7"/>
+      <c r="QA23" s="7"/>
+      <c r="QB23" s="14"/>
+      <c r="QC23" s="22"/>
+      <c r="QD23" s="22"/>
+      <c r="QE23" s="12"/>
+      <c r="QF23" s="16"/>
+      <c r="QG23" s="7"/>
+      <c r="QH23" s="28"/>
+      <c r="QI23" s="14"/>
+      <c r="QJ23" s="11"/>
+      <c r="QK23" s="16"/>
+      <c r="QL23" s="7"/>
+      <c r="QM23" s="28"/>
+      <c r="QN23" s="9"/>
+      <c r="QO23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="QP23" s="12"/>
+      <c r="QQ23" s="20"/>
+      <c r="QR23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="QS23" s="12"/>
+      <c r="QT23" s="12"/>
+      <c r="QU23" s="12"/>
+      <c r="QV23" s="11"/>
+      <c r="QW23" s="11"/>
+      <c r="QX23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="QY23" s="33"/>
+      <c r="QZ23" s="33"/>
+      <c r="RA23" s="33"/>
+      <c r="RB23" s="32"/>
+      <c r="RC23" s="33"/>
+      <c r="RD23" s="20"/>
+      <c r="RE23" s="20"/>
+      <c r="RF23" s="11"/>
+      <c r="RG23" s="20"/>
+      <c r="RH23" s="20"/>
+      <c r="RI23" s="9"/>
+      <c r="RJ23" s="11"/>
+      <c r="RK23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="RL23" s="33"/>
+      <c r="RM23" s="20"/>
+      <c r="RN23" s="11"/>
+      <c r="RO23" s="11"/>
+      <c r="RP23" s="11"/>
+      <c r="RQ23" s="9"/>
+      <c r="RR23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="RS23" s="28"/>
+      <c r="RT23" s="28"/>
+      <c r="RU23" s="7"/>
+      <c r="RW23" s="22"/>
+      <c r="RX23" s="22"/>
+      <c r="RZ23" s="22"/>
+      <c r="SA23" s="12"/>
+      <c r="SB23" s="28"/>
+      <c r="SC23" s="9"/>
+      <c r="SD23" s="9"/>
+      <c r="SF23" s="12"/>
+      <c r="SG23" s="11"/>
+      <c r="SH23" s="11"/>
+      <c r="SI23" s="11"/>
+      <c r="SJ23" s="9"/>
+      <c r="SK23" s="9"/>
+      <c r="SL23" s="16"/>
+      <c r="SM23" s="12"/>
+      <c r="SN23" s="11"/>
+      <c r="SO23" s="11"/>
+      <c r="SP23" s="11"/>
+      <c r="SQ23" s="9"/>
+      <c r="SR23" s="9"/>
+      <c r="SS23" s="16"/>
+      <c r="ST23" s="12"/>
+      <c r="SU23" s="9"/>
+      <c r="SV23" s="12"/>
+      <c r="SW23" s="11"/>
+      <c r="SX23" s="11"/>
+      <c r="SY23" s="11"/>
+      <c r="SZ23" s="13"/>
+      <c r="TA23" s="9"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AU3:AU22 CF3:CF22 DQ3:DQ22 FB3:FB22 GM3:GM22 HX3:HX22 JI3:JI22 KU3:KU22 MN3:MN22 OD3:OD22 QE3:QE22 RT3:RT22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AU3:AU23 CF3:CF23 DQ3:DQ23 FB3:FB23 GM3:GM23 HX3:HX23 JI3:JI23 KU3:KU23 MN3:MN23 OD3:OD23 QE3:QE23 RT3:RT23">
       <formula1>"Normal,OnlyOnce,OnlyOnceDelete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="RX3:RX22">
-      <formula1>'LX ExpeditionZoneData Lists'!$RZ$3:$RZ22</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="RX3:RX23">
+      <formula1>'LX ExpeditionZoneData Lists'!$RZ$3:$RZ23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="R3:R22 BC3:BC22 CN3:CN22 DY3:DY22 FJ3:FJ22 GU3:GU22 IF3:IF22 JR3:JR22 LK3:LK22 MR3:MR22 NA3:NA22 QQ3:QQ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="R3:R23 BC3:BC23 CN3:CN23 DY3:DY23 FJ3:FJ23 GU3:GU23 IF3:IF23 JR3:JR23 LK3:LK23 MR3:MR23 NA3:NA23 QQ3:QQ23">
       <formula1>"Single x1,Single x1_No_close_HUD,Single red x1 No alarm,Checkpoint,Single Small x1,Single Bigger x1,Cluster Small x1,Small Cluster x3 - No Alarm Stealth,Small Cluster x3 - No Alarm Stealth_Far,Small Cluster x2 - No Alarm Stealth,Single D10 req all x1,Team"&amp;" req all x1,single x1 R6A1 Narrative lock,single x1 R6C1 Narrative lock 1,single x1 R6C1 Narrative lock 2,single x1 R6C1 Narrative lock 3,single x1 R6C1 Narrative lock 4,Single x1 - No alarm,HSU_Scan,ExpeditionExit_Scan,ExpeditionExit_Scan_Team,Single x1 "&amp;"- Alarm,Single x1 - Alarm Birther,Single Far x1 - Alarm,Single Far x1 - Alarm Shooters,Single x1 - Alarm Bullrush,Single x1 - Alarm Trickle 2-5,Single x1 - Alarm Trickle 4-6 Bullrush Bigs,Single x2 - Alarm Diminished,Single x2 - Alarm Even More Diminished"&amp;",Single x2 - Alarm Tutorial,Single x2 - Alarm,Single bigger x2 Far - Alarm Halved,Single Bigger x1 Alarm,Single Bigger Separated x2 Alarm,Single Bundled x3 - Alarm,Single x4 - Alarm,Single bigger x3 Far - Alarm,Single bigger x3 Far - Alarm Halved,Single b"&amp;"igger x3 Far - Alarm Halved Bullrush,Single bigger x5  - Alarm,Single Big x6 - Alarm with flyers,Single bigger x4  - Alarm Flyers,Single bigger x5  - Alarm Shadows,Single x1 Moving 58 static points - Alarm,Single x1 Moving 22 static points - Alarm,Single "&amp;"x1 Moving 11 static points - Alarm,Single x1 Moving 3 random points - Alarm Bullrush mix,Single sustained x5 - Alarm Bullrush Mix,Single bigger x1 - Alarm Trickle 2-5,Mixed Separated x3 - Alarm,Mixed Sustained x5 - Alarm Bullrush Mix,Mixed x6 alarm,Mixed "&amp;"x3 - Alarm Diminished,Mixed x4 - Alarm Diminished,Mixed x4 - Alarm Diminished_1AreaSpawn,Mixed x3 - Alarm,Mixed Big x3 - Alarm Reduced Bullrush Mix,Mixed Bundled x3 - Alarm,Mixed x4 - Alarm Halved Bullrush,Mixed x4 Separated - Alarm Shooters,Mixed x4 Sepa"&amp;"rated - Alarm,Mixed x4 - Alarm,Mixed x4 - Alarm Hybrids,Mixed Far x4 - Alarm,Mixed x4 - Alarm Reduced Few Shadows,Mixed x5 - Alarm,Mixed x5 - Alarm Hybrids,Mixed x5 - Alarm_Far,Mixed x5 - Alarm Flyers Spawn Points,Mixed Far Bundled No Req All x5 - Alarm R"&amp;"educed Shadows,Mixed x5 Bundled - Alarm,Mixed Far x5 - Alarm Reduced Bullrush Mix,Mixed Far Separated x5 - Alarm,Mixed Big Cluster Separated x5 - Alarm Hybrids,Mixed x5 - Alarm Diminished,Mixed x5 - Alarm Diminished_Shadows,Mixed x5 - Alarm Diminished_Bul"&amp;"lrush,Mixed Separated x5 - Alarm,Mixed Separated x6 - No alarm,Mixed Separated x5 - Alarm Hybrids,Mixed Separated Far x5 - Alarm Hybrids,Mixed  x6 - Alarm Reduced Bullrush,Mixed Far x6 - Alarm Reduced Bullrush Mix,Mixed Far x6 - Alarm,Mixed Bigs Separated"&amp;" x6 - Alarm Hybrids Modified,Mixed Far Separated x7 - Alarm,Mixed x6 - Alarm Shadows Mixed,Mixed Bigs Separated x4 - Alarm Hybrids,Mixed Far Bundled x3 - Alarm Shadows,Mixed Bundled x3 - Alarm  Reduced Shadows,Mixed Bundled x5 - Alarm Shadows,Mixed Separa"&amp;"ted Far x10 - Alarm,Mixed Separated Far x10 - Alarm_BullRush,Mixed Separated Far x10 - Alarm_Shadows,Mixed Irregular x5 - Alarm Shadows,Mixed Irregular x6 - Alarm Shadows,Mixed Irregular x7 - Alarm Hybrids Modified,Mixed Irregular x5 - Alarm Third Bigs,Mi"&amp;"xed Irregular x7 - Alarm Third Bigs,Mixed Irregular x6 - Alarm Diminished,Mixed Irregular x3 - Alarm Reduced Bullrush Mix,Mixed Irregular x4 - Alarm Reduced Bullrush Mix,Mixed Irregular x4 - Alarm Reduced Bullrush,OLD Chained bioscan mix,Single x1 - Error"&amp;" Alarm Trickle 3-52,Single x1 - Error Alarm Apex Wave From Elevator,Single x1 - Error Alarm Apex Wave From Elevator No Flyers,Single x1 - Error Alarm wave Mainframe,Single x1 - Error Alarm Trickle 4-6 Bullrush Bigs,Single x1 - Error Alarm Trickle 2-45 Bul"&amp;"lrush Bigs,Single x1 - Error Alarm Trickle 3-45 Bullrush Bigs,Single x1 - Error Alarm Trickle 3-30 Hybrids Modified,Single x1 - Error Alarm Trickle 6-30 Shadows,Single x1 - Error Alarm Trickle 4-20 Bullrush,Single x1 - Error Alarm Trickle 5-45 Bullrush,Si"&amp;"ngle x1 - Error Alarm Trickle 4-40 Bigs,Single x1 - Error Alarm Trickle 6-160 Bullrush,Single x1 - Error Alarm Trickle 2-15,Single small x1 - Error Alarm Bullrush Trickle 6-30 Build-up,Single x1 - Error Alarm Big Shadows Trickle 4-60,Single x1 - Error Ala"&amp;"rm Shadows Trickle 8-10 Spawnpoint,Single x1 - Error Alarm Trickle 6-20 From Elevator,Single x1 - Error Alarm Trickle 6-15 Sp-Flyer,Mixed Irregular x4 - Error Alarm Reduced Bullrush Mix,Single Sustained Defend Far x1 - Alarm Diminished,Single Sustained De"&amp;"fend Far x1 - Alarm Increased Hybrids,Single Sustained Defend x1 - Alarm Increased,Single Sustained Defend x1 - Alarm Increased BioscanPoint,Single Sustained Defend x1 - Alarm Increased Further,Single Sustained Defend x1 - Alarm Hybrids Modified,Single Su"&amp;"stained Defend Far x1 - Alarm Hybrids Modifier,Single Sustained Far x3 - Alarm,Single Sustained Far x3 - Alarm Bullrush Miniboss,Single Sustained x4 Far - Alarm,Single Sustained Far x6 - Alarm Increased,Single Sustained x6 - Alarm,Single Sustained Far Bun"&amp;"dled x5 - Alarm Hybrids Modified,Cluster Sustained Far x1 - Alarm,Mixed Sustained Far Separated x3 - Alarm Reduced Bullrush Mix,Cluster x3 - Alarm Diminished Bullrush,Mixed Far Sustained x5 - Alarm Reduced Shadows and Flyers,Mixed Sustained Separated x9 -"&amp;" Diminished Alarm Hybrids,Single Sustained Defend Far x1 - Alarm Surge,Single Sustained Defend MegaHuge x1 - Alarm No Wave,Single Sustained Zone Scan - Alarm 3 sides,Single Sustained Zone Scan - Alarm 3 sides v2,Single Sustained Zone Scan - Alarm Bullrush"&amp;",Single Sustained Zone Scan - Alarm R7D1,Single Sustained Zone Scan - PouncerWaves,Single Sustained Zone Scan No Graphics- Alarm,Single Sustained Defend Huge x1 Alarm Tanks Late,Single Sustained Defend Huge x1 Alarm Birther Late,Cluster x2 - Alarm,Cluster"&amp;" x3 - Alarm,Mixed Cluster big x4 - Alarm,Cluster x3 - Alarm Easier,Cluster x4 - Alarm,Cluster x4 - Alarm - Pouncer,Cluster x5 - Alarm Reduced Bullrush,Cluster x6 - Alarm Reduced Bullrush,Cluster x7 - Alarm Reduced Bullrush,Cluster x7 - Alarm,Cluster x6 - "&amp;"Alarm,Cluster x5 - Alarm,Cluster x5 - Alarm Far,Cluster x4 - Alarm Far,Cluster x4 - Alarm Pretty Far,Cluster x8 - Alarm,Small Cluster x2 - Alarm Shooters,Small Cluster x2 - Alarm Reduced Bullrush,Small Cluster x2 - Alarm,Small Cluster Separated x3 - Alarm"&amp;" Bullrush,Small Cluster Bundled x3 - Alarm,Small Cluster x3 - Alarm Shooters,Small Cluster Separated x3 - Alarm Hybrids Modified,Small Cluster Separated x4 - Alarm,Small Cluster Separated x4 - Alarm Far Diminished,Small Cluster Separated x4 - Alarm Hybrid"&amp;"s,Small Cluster Separated x4 - Alarm Bullrush,Small Cluster Bundled x3 - Alarm_duplicate,Single Far Separated x4 - Alarm Surge,Single Far Separated More x3 - Alarm Surge Hybrids,Mixed Far Separated x3 - Alarm Surge Hybrids,Single Far Separated x4 - Alarm "&amp;"Surge Hybrids,Single Sustained Far Separated x4 - Alarm Surge Hybrids,SecurityScan_Bulkhead_Select_Layer_Main,SecurityScan_Bulkhead_Select_Layer_Secondary,SecurityScan_Bulkhead_Select_Layer_Third"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a EventsOnTrigger and then add it to this Event." sqref="OS3:OS22">
-      <formula1>'LX ExpeditionZoneData Lists'!$JM$3:$JM22</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a EventsOnTrigger and then add it to this Event." sqref="OS3:OS23">
+      <formula1>'LX ExpeditionZoneData Lists'!$JM$3:$JM23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a parsed group and then add it to the log." sqref="QD3:QD22">
-      <formula1>'LX ExpeditionZoneData Lists'!QL$3:QL22</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a parsed group and then add it to the log." sqref="QD3:QD23">
+      <formula1>'LX ExpeditionZoneData Lists'!QL$3:QL23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AN3:AN22 BY3:BY22 DJ3:DJ22 EU3:EU22 GF3:GF22 HQ3:HQ22 JB3:JB22 KN3:KN22 MG3:MG22 NW3:NW22 OO3:OO22 RM3:RM22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AN3:AN23 BY3:BY23 DJ3:DJ23 EU3:EU23 GF3:GF23 HQ3:HQ23 JB3:JB23 KN3:KN23 MG3:MG23 NW3:NW23 OO3:OO23 RM3:RM23">
       <formula1>"Striker_Wave,Striker_Patrol,Striker_Wave_Fast,Striker_Hibernate,Striker_Bullrush,Striker_Big_Wave,Striker_Big_Bullrush,Striker_Big_Hibernate,Striker_Big_Shadow,Striker_Boss,Striker_Child,Shooter_Hibernate,Shooter_Wave,Shooter_Big,Shooter_Big_RapidFire,Sho"&amp;"oter_Big_Infection,Birther,Birther_Boss,Scout,Scout_Bullrush,Scout_Shadow,Cocoon,Shadow,Tank,Tank_Boss,Immortal,Flyer,Flyer_Big,Squidward,SquidBoss_Big,Pouncer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="Q3:Q22 BB3:BB22 CM3:CM22 DX3:DX22 FI3:FI22 GT3:GT22 IE3:IE22 JQ3:JQ22 LJ3:LJ22 MZ3:MZ22 QP3:QP22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="Q3:Q23 BB3:BB23 CM3:CM23 DX3:DX23 FI3:FI23 GT3:GT23 IE3:IE23 JQ3:JQ23 LJ3:LJ23 MZ3:MZ23 QP3:QP23">
       <formula1>"None,OnStart,OnMid,OnEnd"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="OI3:OI22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="OI3:OI23">
       <formula1>"Hibernate,PureSneak,Detect,PureDetect,Patrol,Awake,Hunter"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="PA3:PA22">
-      <formula1>'LX ExpeditionZoneData Lists'!PR$3:PR22</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="PA3:PA23">
+      <formula1>'LX ExpeditionZoneData Lists'!PR$3:PR23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="C3:C22 M3:M22 V3:V22 AX3:AX22 BG3:BG22 CI3:CI22 CR3:CR22 DT3:DT22 EC3:EC22 FE3:FE22 FN3:FN22 GP3:GP22 GY3:GY22 IA3:IA22 IJ3:IJ22 JL3:JL22 JV3:JV22 KX3:KX22 LA3:LA22 LF3:LF22 LO3:LO22 MQ3:MQ22 NE3:NE22 OG3:OG22 ON3:ON22 OQ3:OQ22 OU3:OU22 QU3:QU22 SA3:SA22 SF3:SF22 SM3:SM22 ST3:ST22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="C3:C23 M3:M23 V3:V23 AX3:AX23 BG3:BG23 CI3:CI23 CR3:CR23 DT3:DT23 EC3:EC23 FE3:FE23 FN3:FN23 GP3:GP23 GY3:GY23 IA3:IA23 IJ3:IJ23 JL3:JL23 JV3:JV23 KX3:KX23 LA3:LA23 LF3:LF23 LO3:LO23 MQ3:MQ23 NE3:NE23 OG3:OG23 ON3:ON23 OQ3:OQ23 OU3:OU23 QU3:QU23 SA3:SA23 SF3:SF23 SM3:SM23 ST3:ST23">
       <formula1>"Zone_0,Zone_1,Zone_2,Zone_3,Zone_4,Zone_5,Zone_6,Zone_7,Zone_8,Zone_9,Zone_10,Zone_11,Zone_12,Zone_13,Zone_14,Zone_15,Zone_16,Zone_17,Zone_18,Zone_19,Zone_20"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="PP3:PP22">
-      <formula1>'LX ExpeditionZoneData Lists'!RW$3:RW22</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="PP3:PP23">
+      <formula1>'LX ExpeditionZoneData Lists'!RW$3:RW23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a parsed group and then add it to the log." sqref="QC3:QC22">
-      <formula1>'LX ExpeditionZoneData Lists'!QG$3:QG22</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a parsed group and then add it to the log." sqref="QC3:QC23">
+      <formula1>'LX ExpeditionZoneData Lists'!QG$3:QG23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AE3:AE22 BP3:BP22 DA3:DA22 EL3:EL22 FW3:FW22 HH3:HH22 IS3:IS22 KE3:KE22 LX3:LX22 NN3:NN22 RD3:RD22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AE3:AE23 BP3:BP23 DA3:DA23 EL3:EL23 FW3:FW23 HH3:HH23 IS3:IS23 KE3:KE23 LX3:LX23 NN3:NN23 RD3:RD23">
       <formula1>"low_health_limit,low_health_talk,low_health_grunt,found_health_station_response,oxygen_50,oxygen_25,oxygen_10,oxygen_death,after_damage_fall,on_pick_up_ammo,on_pick_up_health,picked_up_ammo_depleted,on_pick_up_health_when_low,picked_up_keycard_red_a,picke"&amp;"d_up_keycard_blue_a,picked_up_keycard_green_a,picked_up_keycard_yellow_a,picked_up_keycard_white_a,picked_up_keycard_grey_a,picked_up_keycard_black_a,picked_up_keycard_orange_a,picked_up_keycard_purple_a,picked_up_keycard_beige_a,picked_up_keycard_red_b,p"&amp;"icked_up_keycard_blue_b,picked_up_keycard_green_b,picked_up_keycard_yellow_b,picked_up_keycard_white_b,picked_up_keycard_grey_b,picked_up_keycard_black_b,picked_up_keycard_orange_b,picked_up_keycard_purple_b,picked_up_keycard_beige_b,on_ammo_low,ammo_depl"&amp;"eted_reminder,on_reload_weapon_was_out,consumable_depleted_generic,hacking_wrong_first,hacking_wrong_second,hacking_wrong_third,hacking_correct_first,hacking_correct_second,hacking_successful_problematic,hacking_successful_regular,hacking_successful_flawl"&amp;"ess,on_scan_no_enemies,on_scan_few_enemies,on_scan_many_enemies,motion_detector_tagged_plural,on_mapping_finished,cut_lock_first,cut_lock_final,heal_spray_apply_teammate,heal_spray_apply_enemy,sentry_gun_deploy,group_is_not_together,random_comment_pure_st"&amp;"ealth,random_comment_combat_potential,warn_about_tentacles,dark_area_enter,dark_area_light_on,big_space_enter,found_security_post,found_health_station,found_armory,found_scav,found_strongbox,found_resource_box,found_resource_locker,found_meds,found_meds_l"&amp;"ittle,found_ammo,found_ammo_little,idle_no_progress,on_start_open_door,need_keycard_red,need_keycard_blue,need_keycard_green,need_keycard_yellow,need_keycard_white,need_keycard_grey,need_keycard_black,need_keycard_orange,need_keycard_purple,need_keycard_b"&amp;"rown,suggest_keycard_red,suggest_keycard_blue,suggest_keycard_green,suggest_keycard_yellow,suggest_keycard_white,suggest_keycard_grey,suggest_keycard_black,suggest_keycard_orange,suggest_keycard_purple,suggest_keycard_brown,found_node_door,try_to_open_nod"&amp;"e_door,security_door_check,apex_door_to_checkpoint_spot,apex_door_to_elevator_spot,apex_door_fight_anticipation,monster_wave_coming_already_fighting,bio_scan_found,bio_scan_enter,bio_scan_working,generic_done,bio_scan_follow_holo_path,generic_move_to_the_"&amp;"next_one,order_to_bio_scan_woods,order_back_to_bio_scan_woods,order_to_bio_scan_dauda,order_back_to_bio_scan_dauda,order_to_bio_scan_hackett,order_back_to_bio_scan_hackett,order_to_bio_scan_bishop,order_back_to_bio_scan_bishop,accidental_discharge,glottal"&amp;"_stop,caught_by_ceiling_tentacle,land_hard_on_back,shot_yourself_free_from_snatcher,get_shot_free_from_ceiling_tentacle,shoot_parasite_nest,get_parasite,get_parasite_removed,get_parasite_removed_not_all,get_parasite_removed_last,bit_by_parasite,parasite_r"&amp;"emoved_on_teammate,parasite_remove_on_teammate,spot_idle_guard_group,spot_scout,monster_light_sensitivity,killed_single_monster,took_out_scout,attracted_monsters_accident,hear_hunter_group,attracted_monsters_intentional,combat_start,after_damage_generic,a"&amp;"mmo_depleted_taking_damage,man_down_generic,on_char_G_is_downed,on_char_T_is_downed,on_char_F_is_downed,on_char_O_is_downed,help_teammate_up,idle_combat,on_enemy_kill,monsters_breaking_door,monsters_broke_door,friendly_fire_outburst,encounter_over_good,en"&amp;"counter_over_average,encounter_over_bad,encounter_over_scout,on_grabbed_by_tank,held_by_tank,downed_need_help,idle_low_health,death_scream,expedition_start_generic,expedition_start_datamining,expedition_start_scavenge,found_generic_item_1_of_5,found_gener"&amp;"ic_item_2_of_5,found_generic_item_3_of_5,found_generic_item_4_of_5,found_generic_item_final,found_the_item,found_encryption_key_1_of_5,found_encryption_key_2_of_5,found_encryption_key_3_of_5,found_encryption_key_4_of_5,found_encryption_key_final,decon_uni"&amp;"t_briefing,decon_unit_about_to_grab,decon_unit_grabbed,decon_unit_stay_close_reminder,decon_unit_left_behind,get_to_elevator_with_thing,get_to_elevator,get_to_checkpoint_with_thing,get_to_checkpoint,datamining_find_terminal,datamining_found_terminal,datam"&amp;"ining_done_go_to_exit,see_way_to_objective,waypoint_to_data_bank_activated,waypoint_to_checkpoint_activated,waypoint_to_elevator_activated,sneeze,cough_soft,cough_hard,idle_group_bonding,idle_surroundings,just_before_elevator_drop,react_to_woods_log_1,rea"&amp;"ct_to_woods_log_2,react_to_dauda_log_1,react_to_dauda_log_2,react_to_hackett_log_1,react_to_hackett_log_2,react_to_bishop_log_1,react_to_bishop_log_2,ask_for_objective_reminder,find_scav_0,find_scav_1-49,find_scav_50,find_scav_80-99,find_scav_51-79,find_s"&amp;"cav_100,shot_yourself_free_from_ceiling_tentacle,found_item_generic,found_item_succeeding,found_encryption_key_generic,found_encryption_key_succeeding,r06_BigWalkComment,r06_PickUpMWP,r06_TeleportedBackFirstTime,r06_SpotFlyingMonstersFirstTime,r06_Telepor"&amp;"tedMonstersBack,r06_TeleportedFirstTime,CL-Hurry,CL-GoSlow,CL-StandStill,CL-Wait,CL-StayBack,CL-OnMe,CL-North,CL-South,CL-East,CL-West,CL-Left,CL-Right,CL-Middle,CL-FarLeft,CL-FarRight,CL-CheckTheMap,CL-GoQuiet,CL-Shh,CL-WeNeedToPrepare,CL-Synchronize,CL-"&amp;"AreYouReady,CL-ThreeTwoOneGo,CL-GoLoud,CL-BackUp,CL-Scan,CL-WeNeedResources,CL-FocusOnTheObjective,CL-INeedHelp,CL-AlmostThere,CL-Opening,CL-Closing,CL-INeedHealth,CL-MedPackHere,CL-INeedAmmo,CL-AmmoHere,CL-INeedToolRefill,CL-ToolRefillHere,CL-INeedDisinf"&amp;"ection,CL-DisinfectionHere,CL-ResourcesHere,CL-Yes,CL-No,CL-IAgree,CL-IDisagree,CL-Sorry,CL-LetsNotDoThatAgain,CL-WellDone,CL-LotsOfMonstersHere,CL-BigGuyHere,CL-Scout,CL-WeNeedToDoThisTogether,CL-LookUp,CL-RoomClear,CL-Flashlights,CL-IUnderstand,CL-Pleas"&amp;"eRepeatThat,CL-IWillDoIt,CL-NotMe,CL-GrabTheItem,CL-ThisDoor,CL-Terminal,CL-WeNeedATerminal,CL-CFoamHere,CL-TagThem,CL-PutATripmineHere,CL-PutASentryGunHere,CL-ParticleScanHere,CL-WeldThis,CL-NanoSwarmThis,CL-NanoSwarmMe,CL-UseTheNanoSwarm,CL-PickThisUp,C"&amp;"L-ICanDoItShouldI,CL-PickUpYourDeployables,CL-SecureThisRoom,CL-IGotAmmoSomeoneElseCarryThis,CL-Attack,CL-Defend,CL-Please,CL-ThankYou,CL-ImOnMyWay,CL-BRB,CL-CancelThat,CL-Nice,CL-IllTake,CL-YouTake,CL-WeTake,CL-TheOneRightInFrontOfMe,CL-TheOneOnTheRight,"&amp;"CL-TheOneOnTheLeft,CL-TheOneInTheMiddle,CL-TheOneOnTheFarRight,CL-TheOneOnTheFarLeft,CL-TheOneClosestToMe,CL-TheOneClosestToYou,CL-ThisGroup,CL-PickOneEach,CL-LimitedVision,CL-ImExhausted,CL-You,CL-Everyone,CL-Anyone,CL-FollowMe,CL-LetsGTFO,CL-PickUpTheOb"&amp;"jectiveItem,CL-ThrowSomeGlowSticksHere,CL-PutAFogRepellerHere,CL-ICantDoThat,CL-ICantPlaceItThere,CL-IllStayCloseToYou,CL-IllFollowYourLead,CL-ThereAreGlowSticksHere,CL-ThereIsALongRangeFlashlightHere,CL-ThereIsAFogRepellerHere,CL-ThereIsALockMelterHere,C"&amp;"L-ThereIsATripMineHere,CL-ThereIsAFoamMineHere,CL-ThereIsAFoamGrenadeHere,CL-ThereIsARedSyringeHere,CL-ThereIsAYellowSyringeHere,CL-WillDo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="OJ3:OJ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="OJ3:OJ23">
       <formula1>"Easy,Medium,Hard,MiniBoss,Boss,MegaBoss,Biss,Buss"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="OR3:OR22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="OR3:OR23">
       <formula1>"Pickup_PersonnelID,Pickup_PartialDecoder,Pickup_Harddrive,Pickup_GLP-1,Pickup_OSIP,Pickup_GLP-2,Pickup_Data_Cube_Tampered,Pickup_Data_Cube,Pickup_Plant_sample,Pickup_Memory_Stick,Pickup_Memory_Stick_Interactable,Carry_Generator_PowerCell,Carry_HeavyFogRep"&amp;"eller,Carry_HSU_Small_Stage_1,Carry_HSU_Small_Stage_2,Carry_HSU_Small_Stage_3,Carry_HSU_Small_Stage_5,Carry_MWP,Carry_HSU_Small_Stage_4,Carry_DataSphere,Carry_PortalKey,Carry_CargoCrate_Generic,Carry_Cryo_Hardcase,Carry_CargoCrate_HighSecurity,Carry_Cargo"&amp;"Crate_HighSecurity_Open,Carry_Sedatives_Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="N3:N22 AY3:AY22 CJ3:CJ22 DU3:DU22 FF3:FF22 GQ3:GQ22 IB3:IB22 JN3:JN22 LG3:LG22 MW3:MW22 QM3:QM22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="N3:N23 AY3:AY23 CJ3:CJ23 DU3:DU23 FF3:FF23 GQ3:GQ23 IB3:IB23 JN3:JN23 LG3:LG23 MW3:MW23 QM3:QM23">
       <formula1>"None,OpenSecurityDoor,UnlockSecurityDoor,AllLightsOff,AllLightsOn,PlaySound,SetFogSetting,DimensionFlashTeam,DimensionWarpTeam,SpawnEnemyWave,StopEnemyWaves,UpdateCustomSubObjective,ForceCompleteObjective,LightsInZone,LightsInZoneToggle,AnimationTrigger,S"&amp;"pawnEnemyOnPoint,SetNavMarker,StepProgressionObjective,SetWorldEventCondition,LockSecurityDoor,SetTerminalCommand,ActivateChainedPuzzle,EventBreak"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AT3:AT22 CE3:CE22 DP3:DP22 FA3:FA22 GL3:GL22 HW3:HW22 JH3:JH22 KT3:KT22 MM3:MM22 OC3:OC22 RS3:RS22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AT3:AT23 CE3:CE23 DP3:DP23 FA3:FA23 GL3:GL23 HW3:HW23 JH3:JH23 KT3:KT23 MM3:MM23 OC3:OC23 RS3:RS23">
       <formula1>"None,Help,Commands,Cls,Exit,Open,Close,Activate,Deactivate,EmptyLine,InvalidCommand,DownloadData,ViewSecurityLog,Override,DisableAlarm,Locate,ActivateBeacon,Find,ShowList,Query,Ping,ReactorStartup,ReactorVerify,ReactorShutdown,WardenObjectiveSpecialComman"&amp;"d,TerminalUplinkConnect,TerminalUplinkVerify,TerminalUplinkConfirm,ListLogs,ReadLog,Start,TryUnlockingTerminal,WardenObjectiveGatherCommand,TerminalCorruptedUplinkConnect,TerminalCorruptedUplinkVerify,TimedConnectionSend,TimedConnectionVerify,UsedCommand,"&amp;"UniqueCommand1,UniqueCommand2,UniqueCommand3,UniqueCommand4,UniqueCommand5,Info,MAX_COUNT"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="PC3:PC22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="PC3:PC23">
       <formula1>"Sleeping,Awake,PlayerInteracting,DataMining,Hacked,CodePuzzle,InputTest,ReactorError,AskToPlayLogAudio,DoPlayAudioFile,AudioLoopError,Ping,PasswordProtected,EnterPassword"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="PU3:PU22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="PU3:PU23">
       <formula1>"English,French,Italian,German,Spanish,Russian,Portuguese_Brazil,Polish,Japanese,Korean,Chinese_Traditional,Chinese_Simplified"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="QH3:QH22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="QH3:QH23">
       <formula1>"Normal,Fail,SpinningWaitDone,SpinningWaitNoDone,ProgressWait,Warning"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AH3:AH22 BS3:BS22 DD3:DD22 EO3:EO22 FZ3:FZ22 HK3:HK22 IV3:IV22 KH3:KH22 MA3:MA22 NQ3:NQ22 RG3:RG22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AH3:AH23 BS3:BS23 DD3:DD23 EO3:EO23 FZ3:FZ23 HK3:HK23 IV3:IV23 KH3:KH23 MA3:MA23 NQ3:NQ23 RG3:RG23">
       <formula1>"Apex,Apex Tweaked Pop,Apex_SpawnPoints,Apex_Diminished_SpawnPoints,Apex_hack SSpM,Apex No Bigs,Apex No Bigs_Slow,Apex S,Apex WSSpM,Apex WSSpM increased Spawnpoints,Apex Diminished SSp,TimedTerminal 10,Apex Diminished SSp_Delayed,Apex More Diminished SSp,A"&amp;"pex Halved,Apex Halved Standard Only SpawnPoints,Apex Halved SSpMb Only SpawnPoints,Apex Halved And Diminished Standard Only SpawnPoints,Apex Standard Only SpawnPoints,Apex Standard Only Reduced From Elevator,Apex Third,Apex Reduced,Apex Reduced_R7d1,Apex"&amp;" Reduced_Spawnpoints,Apex Reduced_Spawnpoints_R7B3,Apex Reduced W Shadows,Apex Even More Diminished SSp,Apex Reduced Hybrids Mod WSSpM,Apex Increased,Apex Increased SSp,Apex_Fast_from_elevator,Apex_duplicate,Surge,Surge Decreased Groups,Reactor_infiite,De"&amp;"contamination,Scout SSpM,Scout WSSpM,Scout Reduced WSSpM,Scout Halved WSSpM,Scout Halved and Reduced S,Door_wave,Finite 4 S,Finite 1 M,Finite 1 M Spawnpoints,Finite 5 M Spawnpoints,Finite 3 M,Finite 1 1-90 B,Finite 6 3-6 SM,Finite 10 6-10 SM Spawnpoints,F"&amp;"inite WSp_Flyers_Big Spawnpoints,Finite 5 M,Uplink Trickle 5-8 SSp,Uplink Trickle 8-8 WSSpM,Uplink Trickle WSSpM_Flyers,Uplink trickle FogChase WSp_Flyers_Big,Uplink trickle FogChase WSp_Flyers_Small,Trickle 2-5 S,Trickle 2-5 S For Vista,Trickle 2-5 S For"&amp;" Complex,Trickle 1-240 B,Trickle 1-480 MB,Trickle 1-360 MB,Trickle 1-240 MB,Trickle 1-60 MB,Trickle 1-60 TimedTerminal,Trickle 8-360 M,Trickle 8-360 S,Trickle 4-6 B,Trickle 4-20  M,Trickle 6-20 S,Trickle 6-20 S Not From Elevator,Trickle 6-20 SSpMb From El"&amp;"evator,Trickle 6-15 SSpMb,Trickle 8-10 S Spawnpoints,Trickle 4-45 SSpB,Trickle 4-30 SSpB,Trickle 4-30 SSpB_Copy,Trickle 3-30 SSpB,Trickle 6-30 SSpB,Trickle 8-30 SSpB,Trickle 5-45 SpMBB,Trickle 3-180 SpMBB,Trickle 5-30 SSp,Trickle 10-25 SSp,Trickle 10-20 S"&amp;"SpM,Trickle 12-20 SSpM,Trickle 10-20 SSpM Spawnpoints,Trickle 15-20 SSpM,Trickle 14-15 SSpM,Trickle 4-30 SSpM,Trickle 4-28 SSpM,Trickle 4-40 SSpM,Trickle 3-45 SSpB,Trickle 3-70 SSpB,Trickle 3-52 SSpB,Trickle 2-45 S,Trickle 2-60 S,Trickle_6-160 S,Trickle_5"&amp;"-180 S,Trickle 2-15 SSp,Trickle 2-60 MB,Trickle 4-45 MB,Trickle 6-30 SSp,Trickle 2-20  M,Late Trickle 1-60 B,Late Trickle 1-120 B,Exit Trickle 4-10 S,Exit Trickle 10 -40 M,Exit Trickle 4-10 S From Elevator,Exit Trickle 4-10 WSM,Exit Trickle 5-8,Exit Trick"&amp;"le 2-14 SSp,Exit Trickle 3-8 S Original,Exit Trickle 2-12 SSpM,Exit Trickle 2-12 S,Exit Trickle 1-8 S,Shadow Trickle -2- 160 MB From Elevator,Trickle -2- 160 MB,Shadow Trickle -2- 80 SSp From Elevator,Exit Trickle 1-8 S duplicate,Survival phase1,Survival "&amp;"phase1_R7_C3,Survival phase0.5_R7_C3,Survival phase1-5_boss_R7_C3,Survival phase2_7R_C3,Survival phase2-5_boss_R7_C3,Survival phase3_R7_C3,Survival phase3-5_boss_R7_C3,Mainframerush_Standard_wave_Straight_1st,Mainframerush_Standard_wave_Straight_ElevatorP"&amp;"ush,Mainframerush_Standard_wave_Straight_ElevatorPushFromElevator,Mainframerush_Standard_wave_Straight_2nd,Mainframerush_Standard_wave_Straight_3rd,Mainframerush_End_wave_Return,Mainframerush_Modification_End_wave_Return,Mainframerush_Pouncer_End_wave_Ret"&amp;"urn,Mainframerush_Standard_wave_Defence_1st,Mainframerush_Standard_wave_Defence_2nd,Mainframerush_Overload_wave,Mainframerush_Overload_wave_Copy,Mainframerush_Overload_wave_Bigs,MainframeRush_ModificationWave_1st,MainframeRush_ModificationWave_Elevator,Ma"&amp;"inframeRush_ModificationWave_1st_Chicken,MainframeRush_ModificationWave_2nd,MainframeRush_ModificationWave_3rd,MainframeRush_ModificationWave_SidePath_Right,MainframeRush_ModificationWave_SidePath_Left,MainframeRush_ModificationWave_SidePath_1st_Right,Mai"&amp;"nframeRush_ModificationWave_SidePath_1st_Left,MainframeRush_ModificationWave_SidePath_2st_Right,MainframeRush_ModificationWave_SidePath_2st_Left,MainframeRush_ModificationWave_Bigs_Defence_1,MainframeRush_ModificationWave_Bigs_Defence_2,Survival phase4_R7"&amp;"_C3,Survival phase4-5_boss_R7_C3_Pouncer,Survival phase4-5_boss_R7_C3_Big,Survival phase5-5_boss_R7_C3_Hybrids,Survival phase5_R7_C3,Boss_Spawn_Flyer,Survival phase1_6R_C3,Survival phase3_6R_B3,Survival phase2_6R_B3,Survival phase1_6R_B3,PouncerZoneScanWa"&amp;"ves_R7C1,Survival phase3-1_1,Survival phase1-5,Survival phase1-5_6R_C3,Survival phase1-6,Survival phase2,Survival phase2_6R_C3,Survival phase2-2,Survival phase2-5_6R_C3,Survival phase4_6R_C3,Survival phase4_6R_B3,PouncerFinalWaves C1R7,Survival phase3-5_6"&amp;"R_C3,Survival phase3,Survival phase3-1,Survival phase1_boss,Survival phase1_boss_6R_C3,Survival phase1_boss_ext,Survival phase3_boss,Survival phase3_boss_6R_C3,Survival phase3_boss_ext,Survival phase1-5_boss,Survival phase1-5_boss_6R_B3,Survival phase2-5_"&amp;"boss_6R_B3,Reactor 24 SSpMB,Reactor 24 SSpMB Spawnpoints,Reactor 12 SSpMB,Reactor 12 SSpMB Spawnpoints,Reactor 8 SSpMB,Reactor 8 SSpMB Spawnpoints,Reactor 6 SSpMB,Reactor 6 SSpMB Spawnpoints,Reactor 6 MB,Reactor 6 MB Spawnpoints,Reactor 3 MB,Reactor 3 MB "&amp;"Spawnpoints,Reactor 1 MB,Reactor 1 MB Spawnpoints,Flyers_Phase00_wave,Squid_boss,Flyers_Phase01_wave,Flyers_Mainframe,Flyers_Phase02_wave,Flyers_Phase03_wave,Flyers_Phase04_wave,Flyers_Phase05_wave,Flyers_Phase01_rage_wave,Flyers_Phase02_rage_wave,Flyers_"&amp;"Phase03_rage_wave,Flyers_Phase04_rage_wave,Flyers_Phase05_rage_wave,Uplink_WakeUpRunner_Single_MB,Uplink_WakeUpRunner_Single_S"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AF3:AF22 BQ3:BQ22 DB3:DB22 EM3:EM22 FX3:FX22 HI3:HI22 IT3:IT22 KF3:KF22 LY3:LY22 NO3:NO22 RE3:RE22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AF3:AF23 BQ3:BQ23 DB3:DB23 EM3:EM23 FX3:FX23 HI3:HI23 IT3:IT23 KF3:KF23 LY3:LY23 NO3:NO23 RE3:RE23">
       <formula1>"Fog_ELEVATOR,Fog_Mainframe_R7d2,Fog_ELEVATOR_RAIN,desert_fog,desert_fog_sand,Fog_lightest_White_low4_layer,Fog_lightest_White_low_R7B1,Fog_lightest_White_low1_INFECTION,Fog_lightest_White_low1_INFECTION_R6_B2,Fog_lightest_White_low1_INFECTION_R6_D2,Fog_li"&amp;"ght_green_low_INFECTION_R7_B3,Fog_light_green_high_INFECTION_R7_B3,Fog_lightest_White_low1_2_INFECTION,Fog_lightest_White_low1_INFECTION_2,Fog_lightest_White_low1_INFECTION_Copy,Fog_lightest_White_low1_R7C1,Fog_lightest_White_Lowest_1_R7C1,Fog_lightest_Wh"&amp;"ite_low4_layer_Copy,Fog_BX_Dimension,Fog_lightest_White_low4_layer_2,desert_fog_Boss,desert_fog_Boss_Rage,desert_fog_Boss_c1,Fog_lightest_White_low4_layer_2_Copy,Fog_lightest_White_low4_layer_2_fog_in_roof,Fog_lightest_White_low7_layer,Fog_light_white_low"&amp;"6,Fog_light_white_low6_d1,Fog_light_white_low6_d1_Infection,Fog_light_white_low6_Flyer_Arena,Fog_light_white_high_E,Fog_lightest_White_low9_layer,Fog_lightest_White_low9_layer_R4,Fog_very_light_White_low5_layer,Fog_very_light_White_high2_A3_FG_INFECTION,F"&amp;"og_very_light_White_low4_A3_FG_INFECTION,Fog_very_light_White_Low5ToHigh2,Fog_very_light_White_Low5ToHigh2_INFECTION,Fog_very_light_White_Low5ToHigh2_thicker,Fog_very_light_White_High6_thicker_INFECTION,Fog_very_light_White_low_layer,Fog_infectious_R7E1,F"&amp;"og_very_light_White_low_layer_R7B3,Fog_very_light_White_R6D1,Fog_very_light_White_R7D1,Fog_very_light_White_R6D2,Fog_very_light_White_low_layer_thicker,Fog_very_light_White_low_layer_thicker_Copy,Fog_very_light_White_low_dispersed,Fog_very_light_White_low"&amp;"_layer_2,Fog_very_light_White_low3,Fog_light_white_low3,Fog_light_white_low4,Fog_light_white_low_Slow,Fog_light_white_low11,Fog_light_white_high_4,Fog_very_light_White_higher3,Fog_light_green_low2_INFECTION,Fog_light_green_low3_INFECTION,Fog_light_green_l"&amp;"ow3_INFECTION_Copy,Fog_light_green_low0_INFECTION,Fog_light_green_mid0_INFECTION,Fog_light_green_low0_LOW_INFECTION,Fog_light_green_low5_LOW_INFECTION_FG3,Fog_light_green_low6_LOW_INFECTION_FG3,Fog_light_green_low8_INFECTION_R7C2_01,Fog_light_green_high8_"&amp;"INFECTION_R7C2_02,Fog_light_green_high6_INFECTION_R7C2_03_Inverted,Fog_light_green_low2_INFECTION_R7C2_03_Inverted,Fog_light_green_low6_LOW_INFECTION_FG3_R5,Fog_light_green_low6_LOW_INFECTION_R6.5_D4,Fog_light_inverted_mid3_INFECTION,Fog_light_green_inv6_"&amp;"LOW_INFECTION_FG3,Fog_Dimension_MiningShaft_INFECTION,Fog_Dimension_MiningShaft_INFECTION_Copy,Fog_light_green_high1_INFECTION_FG1,Fog_light_green_high1_INFECTION__R6D1,Fog_light_green_high1_INFECTION_FG1_Copy,Fog_light_green_low1_INFECTION_FG1,Fog_light_"&amp;"green_low2_INFECTION_FG1,Fog_light_green_low3_INFECTION_FG1,Fog_light_green_low3_INFECTION_Phase1,Fog_light_green_low3_INFECTION_Phase2,Fog_light_green_low3_INFECTION_Phase3,Fog_light_green_low5_INFECTION_FG1,Fog_light_green_high0_to_3_INFECTION,Fog_light"&amp;"_blue_low1_to_4high_FG1,Fog_light_blue_low9,Fog_light_inverted_high8_FG4,Fog_light_inverted_low2_FG4,Fog_light_low0_INFECTON_FG4,Fog_light_inverted_high8_FG2,Fog_light_inverted_high4_FG2,Fog_light_high2_FG2,Fog_light_high0_FG2,Fog_light_low3_FG2,Fog_light"&amp;"_green_high2_FG5,Fog_light_green_high05_FG5,Fog_light_green_low1_FG5,Fog_light_green_low175_FG5,Fog_light_green_low25_FG5,Fog_light_green_low35_FG5,Fog_light_green_low6_FG5,Fog_light_cyan_alt,Fog_light_white,Fog_light_layered_white,Fog_layered_Infected,Fo"&amp;"g_medium_white,Fog_medium_white_alt,Fog_medium_cyan,Fog_medium_layered_white,Fog_medium_layered_toxic_green,Fog_heavy_layered_light_cyan,Fog_heavy_layered_light_cyan_alt,Fog_light_with_soft_layer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a EventsOnScanDone and then add it to the WorldEventChainedPuzzleDatas." sqref="MT3:MT22">
-      <formula1>'LX ExpeditionZoneData Lists'!MV$3:MV22</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Create a EventsOnScanDone and then add it to the WorldEventChainedPuzzleDatas." sqref="MT3:MT23">
+      <formula1>'LX ExpeditionZoneData Lists'!MV$3:MV23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="SB3:SB22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="SB3:SB23">
       <formula1>"None,SessionSeed,BuildSeed,StaticSeed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="SV3:SV22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="SV3:SV23">
       <formula1>"Weight_is_zeroToOne_startToEnd,Weight_is_exact_node_index"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="T3:T22 BE3:BE22 CP3:CP22 EA3:EA22 FL3:FL22 GW3:GW22 IH3:IH22 JT3:JT22 LM3:LM22 NC3:NC22 QS3:QS22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="T3:T23 BE3:BE23 CP3:CP23 EA3:EA23 FL3:FL23 GW3:GW23 IH3:IH23 JT3:JT23 LM3:LM23 NC3:NC23 QS3:QS23">
       <formula1>"MainLayer,SecondaryLayer,ThirdLayer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AI3:AI22 BT3:BT22 DE3:DE22 EP3:EP22 GA3:GA22 HL3:HL22 IW3:IW22 KI3:KI22 MB3:MB22 NR3:NR22 RH3:RH22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AI3:AI23 BT3:BT23 DE3:DE23 EP3:EP23 GA3:GA23 HL3:HL23 IW3:IW23 KI3:KI23 MB3:MB23 NR3:NR23 RH3:RH23">
       <formula1>"Baseline,Baseline MB-Birther,Baseline MB-Hybrid,Baseline M-Hybrid No Shooter,Baseline M-Bullrush,Baseline Sp-Shadows,Modified Sp-StrikerBig,Modified S-Flyer,Modified S-Flyer_V2,Modified S-Flyer_V3,Modified S-Flyer_V4,Modified Sp-Hybrid,BigsAndBosses,BigsA"&amp;"ndBosses_v2,BigsAndBosses S-Hybrid,BigsAndBosses M-Hybrid,StrikerBigs,Tank,Birther,Bullrush,BullrushBigs,Bullrush_mix,Bullrush_mix6,Bullrush_mix7,Bullrush_mix2,Bullrush_mix3,Bullrush_mix4,Bullrush_mix5,BigsAndHybrid,Baseline Reactor,Baseline Reactor M-Hyb"&amp;"rid,Baseline Reactor S-Child,Shooters,Shadows,Shadows_BigsOnly,Shadows_Sp-Flyer,Flyers,Flyers_Big,Flyers Mb-Flyer Big,Wave_Pouncer,Wave_Pouncer_Combo,Strikers,Boss_FlyerSpawn,Boss_Squid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="PB3:PB22">
-      <formula1>'LX ExpeditionZoneData Lists'!PZ$3:PZ22</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="PB3:PB23">
+      <formula1>'LX ExpeditionZoneData Lists'!PZ$3:PZ23</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="SZ3:SZ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="SZ3:SZ23">
       <formula1>"InfectionSpitter,EggSack_Spreadout,Anemone,Respawner_Sack"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -4294967296 and 4294967295" sqref="A3 O3:O22 AJ3:AJ22 AR3:AR22 AZ3:AZ22 BU3:BU22 CC3:CC22 CK3:CK22 DF3:DF22 DN3:DN22 DV3:DV22 EQ3:EQ22 EY3:EY22 FG3:FG22 GB3:GB22 GJ3:GJ22 GR3:GR22 HM3:HM22 HU3:HU22 IC3:IC22 IX3:IX22 JF3:JF22 JO3:JO22 KJ3:KJ22 KR3:KR22 LH3:LH22 MC3:MC22 MK3:MK22 MX3:MX22 NS3:NS22 OA3:OA22 OY3:OZ22 PM3:PM22 PW3:PW22 QN3:QN22 RI3:RI22 RQ3:RQ22 SC3:SD22 SJ3:SK22 SQ3:SR22 SU3:SU22 TA3:TA22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -4294967296 and 4294967295" sqref="A3 O3:O23 AJ3:AJ23 AR3:AR23 AZ3:AZ23 BU3:BU23 CC3:CC23 CK3:CK23 DF3:DF23 DN3:DN23 DV3:DV23 EQ3:EQ23 EY3:EY23 FG3:FG23 GB3:GB23 GJ3:GJ23 GR3:GR23 HM3:HM23 HU3:HU23 IC3:IC23 IX3:IX23 JF3:JF23 JO3:JO23 KJ3:KJ23 KR3:KR23 LH3:LH23 MC3:MC23 MK3:MK23 MX3:MX23 NS3:NS23 OA3:OA23 OY3:OZ23 PM3:PM23 PW3:PW23 QN3:QN23 RI3:RI23 RQ3:RQ23 SC3:SD23 SJ3:SK23 SQ3:SR23 SU3:SU23 TA3:TA23">
       <formula1>-4.294967296E9</formula1>
       <formula2>4.294967295E9</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="U3:U22 BF3:BF22 CQ3:CQ22 EB3:EB22 FM3:FM22 GX3:GX22 II3:II22 JU3:JU22 KZ3:KZ22 LN3:LN22 ND3:ND22 QT3:QT22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="U3:U23 BF3:BF23 CQ3:CQ23 EB3:EB23 FM3:FM23 GX3:GX23 II3:II23 JU3:JU23 KZ3:KZ23 LN3:LN23 ND3:ND23 QT3:QT23">
       <formula1>"Reality,Dimension_1,Dimension_2,Dimension_3,Dimension_4,Dimension_5,Dimension_6,Dimension_7,Dimension_8,Dimension_9,Dimension_10,Dimension_11,Dimension_12,Dimension_13,Dimension_14,Dimension_15,Dimension_16,Dimension_17,Dimension_18,Dimension_19,Dimension"&amp;"_20,MAX_COUNT,ARENA_DIMENSION"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="D3:D22 F3:G22 W3:X22 AG3:AG22 AK3:AK22 AO3:AQ22 BH3:BI22 BR3:BR22 BV3:BV22 BZ3:CB22 CS3:CT22 DC3:DC22 DG3:DG22 DK3:DM22 ED3:EE22 EN3:EN22 ER3:ER22 EV3:EX22 FO3:FP22 FY3:FY22 GC3:GC22 GG3:GI22 GZ3:HA22 HJ3:HJ22 HN3:HN22 HR3:HT22 IK3:IL22 IU3:IU22 IY3:IY22 JC3:JE22 JW3:JX22 KG3:KG22 KK3:KK22 KO3:KQ22 LB3:LD22 LP3:LQ22 LZ3:LZ22 MD3:MD22 MH3:MJ22 NF3:NG22 NP3:NP22 NT3:NT22 NX3:NZ22 OL3:OL22 OV3:OX22 QJ3:QJ22 QV3:QW22 RF3:RF22 RJ3:RJ22 RN3:RP22 SG3:SI22 SN3:SP22 SW3:SY22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="D3:D23 F3:G23 W3:X23 AG3:AG23 AK3:AK23 AO3:AQ23 BH3:BI23 BR3:BR23 BV3:BV23 BZ3:CB23 CS3:CT23 DC3:DC23 DG3:DG23 DK3:DM23 ED3:EE23 EN3:EN23 ER3:ER23 EV3:EX23 FO3:FP23 FY3:FY23 GC3:GC23 GG3:GI23 GZ3:HA23 HJ3:HJ23 HN3:HN23 HR3:HT23 IK3:IL23 IU3:IU23 IY3:IY23 JC3:JE23 JW3:JX23 KG3:KG23 KK3:KK23 KO3:KQ23 LB3:LD23 LP3:LQ23 LZ3:LZ23 MD3:MD23 MH3:MJ23 NF3:NG23 NP3:NP23 NT3:NT23 NX3:NZ23 OL3:OL23 OV3:OX23 QJ3:QJ23 QV3:QW23 RF3:RF23 RJ3:RJ23 RN3:RP23 SG3:SI23 SN3:SP23 SW3:SY23">
       <formula1>-3.402823E38</formula1>
       <formula2>3.402823E38</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="OK3:OK22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="OK3:OK23">
       <formula1>"None,Force_One,Rel_Value"</formula1>
     </dataValidation>
   </dataValidations>
@@ -34341,55 +35109,259 @@
       <c r="FF22" s="28"/>
       <c r="FG22" s="7"/>
     </row>
+    <row r="23">
+      <c r="A23" s="9">
+        <v>21.0</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="12"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="28"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="28"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="U23" s="12"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="11"/>
+      <c r="AC23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="33"/>
+      <c r="AE23" s="33"/>
+      <c r="AF23" s="33"/>
+      <c r="AG23" s="32"/>
+      <c r="AH23" s="33"/>
+      <c r="AI23" s="20"/>
+      <c r="AJ23" s="20"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="20"/>
+      <c r="AM23" s="20"/>
+      <c r="AN23" s="9"/>
+      <c r="AO23" s="11"/>
+      <c r="AP23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="33"/>
+      <c r="AR23" s="20"/>
+      <c r="AS23" s="11"/>
+      <c r="AT23" s="11"/>
+      <c r="AU23" s="11"/>
+      <c r="AV23" s="9"/>
+      <c r="AW23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="AX23" s="28"/>
+      <c r="AY23" s="28"/>
+      <c r="AZ23" s="7"/>
+      <c r="BB23" s="7"/>
+      <c r="BC23" s="28"/>
+      <c r="BD23" s="9"/>
+      <c r="BE23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BF23" s="12"/>
+      <c r="BG23" s="20"/>
+      <c r="BH23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BI23" s="12"/>
+      <c r="BJ23" s="12"/>
+      <c r="BK23" s="12"/>
+      <c r="BL23" s="11"/>
+      <c r="BM23" s="11"/>
+      <c r="BN23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="BO23" s="33"/>
+      <c r="BP23" s="33"/>
+      <c r="BQ23" s="33"/>
+      <c r="BR23" s="32"/>
+      <c r="BS23" s="33"/>
+      <c r="BT23" s="20"/>
+      <c r="BU23" s="20"/>
+      <c r="BV23" s="11"/>
+      <c r="BW23" s="20"/>
+      <c r="BX23" s="20"/>
+      <c r="BY23" s="9"/>
+      <c r="BZ23" s="11"/>
+      <c r="CA23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CB23" s="33"/>
+      <c r="CC23" s="20"/>
+      <c r="CD23" s="11"/>
+      <c r="CE23" s="11"/>
+      <c r="CF23" s="11"/>
+      <c r="CG23" s="9"/>
+      <c r="CH23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CI23" s="28"/>
+      <c r="CJ23" s="28"/>
+      <c r="CK23" s="7"/>
+      <c r="CM23" s="7"/>
+      <c r="CN23" s="28"/>
+      <c r="CO23" s="9"/>
+      <c r="CP23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CQ23" s="12"/>
+      <c r="CR23" s="20"/>
+      <c r="CS23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CT23" s="12"/>
+      <c r="CU23" s="12"/>
+      <c r="CV23" s="12"/>
+      <c r="CW23" s="11"/>
+      <c r="CX23" s="11"/>
+      <c r="CY23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="CZ23" s="33"/>
+      <c r="DA23" s="33"/>
+      <c r="DB23" s="33"/>
+      <c r="DC23" s="32"/>
+      <c r="DD23" s="33"/>
+      <c r="DE23" s="20"/>
+      <c r="DF23" s="20"/>
+      <c r="DG23" s="11"/>
+      <c r="DH23" s="20"/>
+      <c r="DI23" s="20"/>
+      <c r="DJ23" s="9"/>
+      <c r="DK23" s="11"/>
+      <c r="DL23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="DM23" s="33"/>
+      <c r="DN23" s="20"/>
+      <c r="DO23" s="11"/>
+      <c r="DP23" s="11"/>
+      <c r="DQ23" s="11"/>
+      <c r="DR23" s="9"/>
+      <c r="DS23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="DT23" s="28"/>
+      <c r="DU23" s="28"/>
+      <c r="DV23" s="7"/>
+      <c r="DX23" s="7"/>
+      <c r="DY23" s="28"/>
+      <c r="DZ23" s="9"/>
+      <c r="EA23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="EB23" s="12"/>
+      <c r="EC23" s="20"/>
+      <c r="ED23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="EE23" s="12"/>
+      <c r="EF23" s="12"/>
+      <c r="EG23" s="12"/>
+      <c r="EH23" s="11"/>
+      <c r="EI23" s="11"/>
+      <c r="EJ23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="EK23" s="33"/>
+      <c r="EL23" s="33"/>
+      <c r="EM23" s="33"/>
+      <c r="EN23" s="32"/>
+      <c r="EO23" s="33"/>
+      <c r="EP23" s="20"/>
+      <c r="EQ23" s="20"/>
+      <c r="ER23" s="11"/>
+      <c r="ES23" s="20"/>
+      <c r="ET23" s="20"/>
+      <c r="EU23" s="9"/>
+      <c r="EV23" s="11"/>
+      <c r="EW23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="EX23" s="33"/>
+      <c r="EY23" s="20"/>
+      <c r="EZ23" s="11"/>
+      <c r="FA23" s="11"/>
+      <c r="FB23" s="11"/>
+      <c r="FC23" s="9"/>
+      <c r="FD23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="FE23" s="28"/>
+      <c r="FF23" s="28"/>
+      <c r="FG23" s="7"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AY3:AY22 CJ3:CJ22 DU3:DU22 FF3:FF22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AY3:AY23 CJ3:CJ23 DU3:DU23 FF3:FF23">
       <formula1>"Normal,OnlyOnce,OnlyOnceDelete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="V3:V22 BG3:BG22 CR3:CR22 EC3:EC22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="V3:V23 BG3:BG23 CR3:CR23 EC3:EC23">
       <formula1>"Single x1,Single x1_No_close_HUD,Single red x1 No alarm,Checkpoint,Single Small x1,Single Bigger x1,Cluster Small x1,Small Cluster x3 - No Alarm Stealth,Small Cluster x3 - No Alarm Stealth_Far,Small Cluster x2 - No Alarm Stealth,Single D10 req all x1,Team"&amp;" req all x1,single x1 R6A1 Narrative lock,single x1 R6C1 Narrative lock 1,single x1 R6C1 Narrative lock 2,single x1 R6C1 Narrative lock 3,single x1 R6C1 Narrative lock 4,Single x1 - No alarm,HSU_Scan,ExpeditionExit_Scan,ExpeditionExit_Scan_Team,Single x1 "&amp;"- Alarm,Single x1 - Alarm Birther,Single Far x1 - Alarm,Single Far x1 - Alarm Shooters,Single x1 - Alarm Bullrush,Single x1 - Alarm Trickle 2-5,Single x1 - Alarm Trickle 4-6 Bullrush Bigs,Single x2 - Alarm Diminished,Single x2 - Alarm Even More Diminished"&amp;",Single x2 - Alarm Tutorial,Single x2 - Alarm,Single bigger x2 Far - Alarm Halved,Single Bigger x1 Alarm,Single Bigger Separated x2 Alarm,Single Bundled x3 - Alarm,Single x4 - Alarm,Single bigger x3 Far - Alarm,Single bigger x3 Far - Alarm Halved,Single b"&amp;"igger x3 Far - Alarm Halved Bullrush,Single bigger x5  - Alarm,Single Big x6 - Alarm with flyers,Single bigger x4  - Alarm Flyers,Single bigger x5  - Alarm Shadows,Single x1 Moving 58 static points - Alarm,Single x1 Moving 22 static points - Alarm,Single "&amp;"x1 Moving 11 static points - Alarm,Single x1 Moving 3 random points - Alarm Bullrush mix,Single sustained x5 - Alarm Bullrush Mix,Single bigger x1 - Alarm Trickle 2-5,Mixed Separated x3 - Alarm,Mixed Sustained x5 - Alarm Bullrush Mix,Mixed x6 alarm,Mixed "&amp;"x3 - Alarm Diminished,Mixed x4 - Alarm Diminished,Mixed x4 - Alarm Diminished_1AreaSpawn,Mixed x3 - Alarm,Mixed Big x3 - Alarm Reduced Bullrush Mix,Mixed Bundled x3 - Alarm,Mixed x4 - Alarm Halved Bullrush,Mixed x4 Separated - Alarm Shooters,Mixed x4 Sepa"&amp;"rated - Alarm,Mixed x4 - Alarm,Mixed x4 - Alarm Hybrids,Mixed Far x4 - Alarm,Mixed x4 - Alarm Reduced Few Shadows,Mixed x5 - Alarm,Mixed x5 - Alarm Hybrids,Mixed x5 - Alarm_Far,Mixed x5 - Alarm Flyers Spawn Points,Mixed Far Bundled No Req All x5 - Alarm R"&amp;"educed Shadows,Mixed x5 Bundled - Alarm,Mixed Far x5 - Alarm Reduced Bullrush Mix,Mixed Far Separated x5 - Alarm,Mixed Big Cluster Separated x5 - Alarm Hybrids,Mixed x5 - Alarm Diminished,Mixed x5 - Alarm Diminished_Shadows,Mixed x5 - Alarm Diminished_Bul"&amp;"lrush,Mixed Separated x5 - Alarm,Mixed Separated x6 - No alarm,Mixed Separated x5 - Alarm Hybrids,Mixed Separated Far x5 - Alarm Hybrids,Mixed  x6 - Alarm Reduced Bullrush,Mixed Far x6 - Alarm Reduced Bullrush Mix,Mixed Far x6 - Alarm,Mixed Bigs Separated"&amp;" x6 - Alarm Hybrids Modified,Mixed Far Separated x7 - Alarm,Mixed x6 - Alarm Shadows Mixed,Mixed Bigs Separated x4 - Alarm Hybrids,Mixed Far Bundled x3 - Alarm Shadows,Mixed Bundled x3 - Alarm  Reduced Shadows,Mixed Bundled x5 - Alarm Shadows,Mixed Separa"&amp;"ted Far x10 - Alarm,Mixed Separated Far x10 - Alarm_BullRush,Mixed Separated Far x10 - Alarm_Shadows,Mixed Irregular x5 - Alarm Shadows,Mixed Irregular x6 - Alarm Shadows,Mixed Irregular x7 - Alarm Hybrids Modified,Mixed Irregular x5 - Alarm Third Bigs,Mi"&amp;"xed Irregular x7 - Alarm Third Bigs,Mixed Irregular x6 - Alarm Diminished,Mixed Irregular x3 - Alarm Reduced Bullrush Mix,Mixed Irregular x4 - Alarm Reduced Bullrush Mix,Mixed Irregular x4 - Alarm Reduced Bullrush,OLD Chained bioscan mix,Single x1 - Error"&amp;" Alarm Trickle 3-52,Single x1 - Error Alarm Apex Wave From Elevator,Single x1 - Error Alarm Apex Wave From Elevator No Flyers,Single x1 - Error Alarm wave Mainframe,Single x1 - Error Alarm Trickle 4-6 Bullrush Bigs,Single x1 - Error Alarm Trickle 2-45 Bul"&amp;"lrush Bigs,Single x1 - Error Alarm Trickle 3-45 Bullrush Bigs,Single x1 - Error Alarm Trickle 3-30 Hybrids Modified,Single x1 - Error Alarm Trickle 6-30 Shadows,Single x1 - Error Alarm Trickle 4-20 Bullrush,Single x1 - Error Alarm Trickle 5-45 Bullrush,Si"&amp;"ngle x1 - Error Alarm Trickle 4-40 Bigs,Single x1 - Error Alarm Trickle 6-160 Bullrush,Single x1 - Error Alarm Trickle 2-15,Single small x1 - Error Alarm Bullrush Trickle 6-30 Build-up,Single x1 - Error Alarm Big Shadows Trickle 4-60,Single x1 - Error Ala"&amp;"rm Shadows Trickle 8-10 Spawnpoint,Single x1 - Error Alarm Trickle 6-20 From Elevator,Single x1 - Error Alarm Trickle 6-15 Sp-Flyer,Mixed Irregular x4 - Error Alarm Reduced Bullrush Mix,Single Sustained Defend Far x1 - Alarm Diminished,Single Sustained De"&amp;"fend Far x1 - Alarm Increased Hybrids,Single Sustained Defend x1 - Alarm Increased,Single Sustained Defend x1 - Alarm Increased BioscanPoint,Single Sustained Defend x1 - Alarm Increased Further,Single Sustained Defend x1 - Alarm Hybrids Modified,Single Su"&amp;"stained Defend Far x1 - Alarm Hybrids Modifier,Single Sustained Far x3 - Alarm,Single Sustained Far x3 - Alarm Bullrush Miniboss,Single Sustained x4 Far - Alarm,Single Sustained Far x6 - Alarm Increased,Single Sustained x6 - Alarm,Single Sustained Far Bun"&amp;"dled x5 - Alarm Hybrids Modified,Cluster Sustained Far x1 - Alarm,Mixed Sustained Far Separated x3 - Alarm Reduced Bullrush Mix,Cluster x3 - Alarm Diminished Bullrush,Mixed Far Sustained x5 - Alarm Reduced Shadows and Flyers,Mixed Sustained Separated x9 -"&amp;" Diminished Alarm Hybrids,Single Sustained Defend Far x1 - Alarm Surge,Single Sustained Defend MegaHuge x1 - Alarm No Wave,Single Sustained Zone Scan - Alarm 3 sides,Single Sustained Zone Scan - Alarm 3 sides v2,Single Sustained Zone Scan - Alarm Bullrush"&amp;",Single Sustained Zone Scan - Alarm R7D1,Single Sustained Zone Scan - PouncerWaves,Single Sustained Zone Scan No Graphics- Alarm,Single Sustained Defend Huge x1 Alarm Tanks Late,Single Sustained Defend Huge x1 Alarm Birther Late,Cluster x2 - Alarm,Cluster"&amp;" x3 - Alarm,Mixed Cluster big x4 - Alarm,Cluster x3 - Alarm Easier,Cluster x4 - Alarm,Cluster x4 - Alarm - Pouncer,Cluster x5 - Alarm Reduced Bullrush,Cluster x6 - Alarm Reduced Bullrush,Cluster x7 - Alarm Reduced Bullrush,Cluster x7 - Alarm,Cluster x6 - "&amp;"Alarm,Cluster x5 - Alarm,Cluster x5 - Alarm Far,Cluster x4 - Alarm Far,Cluster x4 - Alarm Pretty Far,Cluster x8 - Alarm,Small Cluster x2 - Alarm Shooters,Small Cluster x2 - Alarm Reduced Bullrush,Small Cluster x2 - Alarm,Small Cluster Separated x3 - Alarm"&amp;" Bullrush,Small Cluster Bundled x3 - Alarm,Small Cluster x3 - Alarm Shooters,Small Cluster Separated x3 - Alarm Hybrids Modified,Small Cluster Separated x4 - Alarm,Small Cluster Separated x4 - Alarm Far Diminished,Small Cluster Separated x4 - Alarm Hybrid"&amp;"s,Small Cluster Separated x4 - Alarm Bullrush,Small Cluster Bundled x3 - Alarm_duplicate,Single Far Separated x4 - Alarm Surge,Single Far Separated More x3 - Alarm Surge Hybrids,Mixed Far Separated x3 - Alarm Surge Hybrids,Single Far Separated x4 - Alarm "&amp;"Surge Hybrids,Single Sustained Far Separated x4 - Alarm Surge Hybrids,SecurityScan_Bulkhead_Select_Layer_Main,SecurityScan_Bulkhead_Select_Layer_Secondary,SecurityScan_Bulkhead_Select_Layer_Third"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="K3:K22 AL3:AL22 BW3:BW22 DH3:DH22 ES3:ES22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="K3:K23 AL3:AL23 BW3:BW23 DH3:DH23 ES3:ES23">
       <formula1>"Apex,Apex Tweaked Pop,Apex_SpawnPoints,Apex_Diminished_SpawnPoints,Apex_hack SSpM,Apex No Bigs,Apex No Bigs_Slow,Apex S,Apex WSSpM,Apex WSSpM increased Spawnpoints,Apex Diminished SSp,TimedTerminal 10,Apex Diminished SSp_Delayed,Apex More Diminished SSp,A"&amp;"pex Halved,Apex Halved Standard Only SpawnPoints,Apex Halved SSpMb Only SpawnPoints,Apex Halved And Diminished Standard Only SpawnPoints,Apex Standard Only SpawnPoints,Apex Standard Only Reduced From Elevator,Apex Third,Apex Reduced,Apex Reduced_R7d1,Apex"&amp;" Reduced_Spawnpoints,Apex Reduced_Spawnpoints_R7B3,Apex Reduced W Shadows,Apex Even More Diminished SSp,Apex Reduced Hybrids Mod WSSpM,Apex Increased,Apex Increased SSp,Apex_Fast_from_elevator,Apex_duplicate,Surge,Surge Decreased Groups,Reactor_infiite,De"&amp;"contamination,Scout SSpM,Scout WSSpM,Scout Reduced WSSpM,Scout Halved WSSpM,Scout Halved and Reduced S,Door_wave,Finite 4 S,Finite 1 M,Finite 1 M Spawnpoints,Finite 5 M Spawnpoints,Finite 3 M,Finite 1 1-90 B,Finite 6 3-6 SM,Finite 10 6-10 SM Spawnpoints,F"&amp;"inite WSp_Flyers_Big Spawnpoints,Finite 5 M,Uplink Trickle 5-8 SSp,Uplink Trickle 8-8 WSSpM,Uplink Trickle WSSpM_Flyers,Uplink trickle FogChase WSp_Flyers_Big,Uplink trickle FogChase WSp_Flyers_Small,Trickle 2-5 S,Trickle 2-5 S For Vista,Trickle 2-5 S For"&amp;" Complex,Trickle 1-240 B,Trickle 1-480 MB,Trickle 1-360 MB,Trickle 1-240 MB,Trickle 1-60 MB,Trickle 1-60 TimedTerminal,Trickle 8-360 M,Trickle 8-360 S,Trickle 4-6 B,Trickle 4-20  M,Trickle 6-20 S,Trickle 6-20 S Not From Elevator,Trickle 6-20 SSpMb From El"&amp;"evator,Trickle 6-15 SSpMb,Trickle 8-10 S Spawnpoints,Trickle 4-45 SSpB,Trickle 4-30 SSpB,Trickle 4-30 SSpB_Copy,Trickle 3-30 SSpB,Trickle 6-30 SSpB,Trickle 8-30 SSpB,Trickle 5-45 SpMBB,Trickle 3-180 SpMBB,Trickle 5-30 SSp,Trickle 10-25 SSp,Trickle 10-20 S"&amp;"SpM,Trickle 12-20 SSpM,Trickle 10-20 SSpM Spawnpoints,Trickle 15-20 SSpM,Trickle 14-15 SSpM,Trickle 4-30 SSpM,Trickle 4-28 SSpM,Trickle 4-40 SSpM,Trickle 3-45 SSpB,Trickle 3-70 SSpB,Trickle 3-52 SSpB,Trickle 2-45 S,Trickle 2-60 S,Trickle_6-160 S,Trickle_5"&amp;"-180 S,Trickle 2-15 SSp,Trickle 2-60 MB,Trickle 4-45 MB,Trickle 6-30 SSp,Trickle 2-20  M,Late Trickle 1-60 B,Late Trickle 1-120 B,Exit Trickle 4-10 S,Exit Trickle 10 -40 M,Exit Trickle 4-10 S From Elevator,Exit Trickle 4-10 WSM,Exit Trickle 5-8,Exit Trick"&amp;"le 2-14 SSp,Exit Trickle 3-8 S Original,Exit Trickle 2-12 SSpM,Exit Trickle 2-12 S,Exit Trickle 1-8 S,Shadow Trickle -2- 160 MB From Elevator,Trickle -2- 160 MB,Shadow Trickle -2- 80 SSp From Elevator,Exit Trickle 1-8 S duplicate,Survival phase1,Survival "&amp;"phase1_R7_C3,Survival phase0.5_R7_C3,Survival phase1-5_boss_R7_C3,Survival phase2_7R_C3,Survival phase2-5_boss_R7_C3,Survival phase3_R7_C3,Survival phase3-5_boss_R7_C3,Mainframerush_Standard_wave_Straight_1st,Mainframerush_Standard_wave_Straight_ElevatorP"&amp;"ush,Mainframerush_Standard_wave_Straight_ElevatorPushFromElevator,Mainframerush_Standard_wave_Straight_2nd,Mainframerush_Standard_wave_Straight_3rd,Mainframerush_End_wave_Return,Mainframerush_Modification_End_wave_Return,Mainframerush_Pouncer_End_wave_Ret"&amp;"urn,Mainframerush_Standard_wave_Defence_1st,Mainframerush_Standard_wave_Defence_2nd,Mainframerush_Overload_wave,Mainframerush_Overload_wave_Copy,Mainframerush_Overload_wave_Bigs,MainframeRush_ModificationWave_1st,MainframeRush_ModificationWave_Elevator,Ma"&amp;"inframeRush_ModificationWave_1st_Chicken,MainframeRush_ModificationWave_2nd,MainframeRush_ModificationWave_3rd,MainframeRush_ModificationWave_SidePath_Right,MainframeRush_ModificationWave_SidePath_Left,MainframeRush_ModificationWave_SidePath_1st_Right,Mai"&amp;"nframeRush_ModificationWave_SidePath_1st_Left,MainframeRush_ModificationWave_SidePath_2st_Right,MainframeRush_ModificationWave_SidePath_2st_Left,MainframeRush_ModificationWave_Bigs_Defence_1,MainframeRush_ModificationWave_Bigs_Defence_2,Survival phase4_R7"&amp;"_C3,Survival phase4-5_boss_R7_C3_Pouncer,Survival phase4-5_boss_R7_C3_Big,Survival phase5-5_boss_R7_C3_Hybrids,Survival phase5_R7_C3,Boss_Spawn_Flyer,Survival phase1_6R_C3,Survival phase3_6R_B3,Survival phase2_6R_B3,Survival phase1_6R_B3,PouncerZoneScanWa"&amp;"ves_R7C1,Survival phase3-1_1,Survival phase1-5,Survival phase1-5_6R_C3,Survival phase1-6,Survival phase2,Survival phase2_6R_C3,Survival phase2-2,Survival phase2-5_6R_C3,Survival phase4_6R_C3,Survival phase4_6R_B3,PouncerFinalWaves C1R7,Survival phase3-5_6"&amp;"R_C3,Survival phase3,Survival phase3-1,Survival phase1_boss,Survival phase1_boss_6R_C3,Survival phase1_boss_ext,Survival phase3_boss,Survival phase3_boss_6R_C3,Survival phase3_boss_ext,Survival phase1-5_boss,Survival phase1-5_boss_6R_B3,Survival phase2-5_"&amp;"boss_6R_B3,Reactor 24 SSpMB,Reactor 24 SSpMB Spawnpoints,Reactor 12 SSpMB,Reactor 12 SSpMB Spawnpoints,Reactor 8 SSpMB,Reactor 8 SSpMB Spawnpoints,Reactor 6 SSpMB,Reactor 6 SSpMB Spawnpoints,Reactor 6 MB,Reactor 6 MB Spawnpoints,Reactor 3 MB,Reactor 3 MB "&amp;"Spawnpoints,Reactor 1 MB,Reactor 1 MB Spawnpoints,Flyers_Phase00_wave,Squid_boss,Flyers_Phase01_wave,Flyers_Mainframe,Flyers_Phase02_wave,Flyers_Phase03_wave,Flyers_Phase04_wave,Flyers_Phase05_wave,Flyers_Phase01_rage_wave,Flyers_Phase02_rage_wave,Flyers_"&amp;"Phase03_rage_wave,Flyers_Phase04_rage_wave,Flyers_Phase05_rage_wave,Uplink_WakeUpRunner_Single_MB,Uplink_WakeUpRunner_Single_S"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AR3:AR22 CC3:CC22 DN3:DN22 EY3:EY22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AR3:AR23 CC3:CC23 DN3:DN23 EY3:EY23">
       <formula1>"Striker_Wave,Striker_Patrol,Striker_Wave_Fast,Striker_Hibernate,Striker_Bullrush,Striker_Big_Wave,Striker_Big_Bullrush,Striker_Big_Hibernate,Striker_Big_Shadow,Striker_Boss,Striker_Child,Shooter_Hibernate,Shooter_Wave,Shooter_Big,Shooter_Big_RapidFire,Sho"&amp;"oter_Big_Infection,Birther,Birther_Boss,Scout,Scout_Bullrush,Scout_Shadow,Cocoon,Shadow,Tank,Tank_Boss,Immortal,Flyer,Flyer_Big,Squidward,SquidBoss_Big,Pouncer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AJ3:AJ22 BU3:BU22 DF3:DF22 EQ3:EQ22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AJ3:AJ23 BU3:BU23 DF3:DF23 EQ3:EQ23">
       <formula1>"Fog_ELEVATOR,Fog_Mainframe_R7d2,Fog_ELEVATOR_RAIN,desert_fog,desert_fog_sand,Fog_lightest_White_low4_layer,Fog_lightest_White_low_R7B1,Fog_lightest_White_low1_INFECTION,Fog_lightest_White_low1_INFECTION_R6_B2,Fog_lightest_White_low1_INFECTION_R6_D2,Fog_li"&amp;"ght_green_low_INFECTION_R7_B3,Fog_light_green_high_INFECTION_R7_B3,Fog_lightest_White_low1_2_INFECTION,Fog_lightest_White_low1_INFECTION_2,Fog_lightest_White_low1_INFECTION_Copy,Fog_lightest_White_low1_R7C1,Fog_lightest_White_Lowest_1_R7C1,Fog_lightest_Wh"&amp;"ite_low4_layer_Copy,Fog_BX_Dimension,Fog_lightest_White_low4_layer_2,desert_fog_Boss,desert_fog_Boss_Rage,desert_fog_Boss_c1,Fog_lightest_White_low4_layer_2_Copy,Fog_lightest_White_low4_layer_2_fog_in_roof,Fog_lightest_White_low7_layer,Fog_light_white_low"&amp;"6,Fog_light_white_low6_d1,Fog_light_white_low6_d1_Infection,Fog_light_white_low6_Flyer_Arena,Fog_light_white_high_E,Fog_lightest_White_low9_layer,Fog_lightest_White_low9_layer_R4,Fog_very_light_White_low5_layer,Fog_very_light_White_high2_A3_FG_INFECTION,F"&amp;"og_very_light_White_low4_A3_FG_INFECTION,Fog_very_light_White_Low5ToHigh2,Fog_very_light_White_Low5ToHigh2_INFECTION,Fog_very_light_White_Low5ToHigh2_thicker,Fog_very_light_White_High6_thicker_INFECTION,Fog_very_light_White_low_layer,Fog_infectious_R7E1,F"&amp;"og_very_light_White_low_layer_R7B3,Fog_very_light_White_R6D1,Fog_very_light_White_R7D1,Fog_very_light_White_R6D2,Fog_very_light_White_low_layer_thicker,Fog_very_light_White_low_layer_thicker_Copy,Fog_very_light_White_low_dispersed,Fog_very_light_White_low"&amp;"_layer_2,Fog_very_light_White_low3,Fog_light_white_low3,Fog_light_white_low4,Fog_light_white_low_Slow,Fog_light_white_low11,Fog_light_white_high_4,Fog_very_light_White_higher3,Fog_light_green_low2_INFECTION,Fog_light_green_low3_INFECTION,Fog_light_green_l"&amp;"ow3_INFECTION_Copy,Fog_light_green_low0_INFECTION,Fog_light_green_mid0_INFECTION,Fog_light_green_low0_LOW_INFECTION,Fog_light_green_low5_LOW_INFECTION_FG3,Fog_light_green_low6_LOW_INFECTION_FG3,Fog_light_green_low8_INFECTION_R7C2_01,Fog_light_green_high8_"&amp;"INFECTION_R7C2_02,Fog_light_green_high6_INFECTION_R7C2_03_Inverted,Fog_light_green_low2_INFECTION_R7C2_03_Inverted,Fog_light_green_low6_LOW_INFECTION_FG3_R5,Fog_light_green_low6_LOW_INFECTION_R6.5_D4,Fog_light_inverted_mid3_INFECTION,Fog_light_green_inv6_"&amp;"LOW_INFECTION_FG3,Fog_Dimension_MiningShaft_INFECTION,Fog_Dimension_MiningShaft_INFECTION_Copy,Fog_light_green_high1_INFECTION_FG1,Fog_light_green_high1_INFECTION__R6D1,Fog_light_green_high1_INFECTION_FG1_Copy,Fog_light_green_low1_INFECTION_FG1,Fog_light_"&amp;"green_low2_INFECTION_FG1,Fog_light_green_low3_INFECTION_FG1,Fog_light_green_low3_INFECTION_Phase1,Fog_light_green_low3_INFECTION_Phase2,Fog_light_green_low3_INFECTION_Phase3,Fog_light_green_low5_INFECTION_FG1,Fog_light_green_high0_to_3_INFECTION,Fog_light"&amp;"_blue_low1_to_4high_FG1,Fog_light_blue_low9,Fog_light_inverted_high8_FG4,Fog_light_inverted_low2_FG4,Fog_light_low0_INFECTON_FG4,Fog_light_inverted_high8_FG2,Fog_light_inverted_high4_FG2,Fog_light_high2_FG2,Fog_light_high0_FG2,Fog_light_low3_FG2,Fog_light"&amp;"_green_high2_FG5,Fog_light_green_high05_FG5,Fog_light_green_low1_FG5,Fog_light_green_low175_FG5,Fog_light_green_low25_FG5,Fog_light_green_low35_FG5,Fog_light_green_low6_FG5,Fog_light_cyan_alt,Fog_light_white,Fog_light_layered_white,Fog_layered_Infected,Fo"&amp;"g_medium_white,Fog_medium_white_alt,Fog_medium_cyan,Fog_medium_layered_white,Fog_medium_layered_toxic_green,Fog_heavy_layered_light_cyan,Fog_heavy_layered_light_cyan_alt,Fog_light_with_soft_layer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="U3:U22 BF3:BF22 CQ3:CQ22 EB3:EB22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="U3:U23 BF3:BF23 CQ3:CQ23 EB3:EB23">
       <formula1>"None,OnStart,OnMid,OnEnd"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="L3:L22 AM3:AM22 BX3:BX22 DI3:DI22 ET3:ET22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="L3:L23 AM3:AM23 BX3:BX23 DI3:DI23 ET3:ET23">
       <formula1>"Baseline,Baseline MB-Birther,Baseline MB-Hybrid,Baseline M-Hybrid No Shooter,Baseline M-Bullrush,Baseline Sp-Shadows,Modified Sp-StrikerBig,Modified S-Flyer,Modified S-Flyer_V2,Modified S-Flyer_V3,Modified S-Flyer_V4,Modified Sp-Hybrid,BigsAndBosses,BigsA"&amp;"ndBosses_v2,BigsAndBosses S-Hybrid,BigsAndBosses M-Hybrid,StrikerBigs,Tank,Birther,Bullrush,BullrushBigs,Bullrush_mix,Bullrush_mix6,Bullrush_mix7,Bullrush_mix2,Bullrush_mix3,Bullrush_mix4,Bullrush_mix5,BigsAndHybrid,Baseline Reactor,Baseline Reactor M-Hyb"&amp;"rid,Baseline Reactor S-Child,Shooters,Shadows,Shadows_BigsOnly,Shadows_Sp-Flyer,Flyers,Flyers_Big,Flyers Mb-Flyer Big,Wave_Pouncer,Wave_Pouncer_Combo,Strikers,Boss_FlyerSpawn,Boss_Squid"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="X3:X22 BI3:BI22 CT3:CT22 EE3:EE22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="X3:X23 BI3:BI23 CT3:CT23 EE3:EE23">
       <formula1>"MainLayer,SecondaryLayer,ThirdLayer"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="O3:O22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="O3:O23">
       <formula1>"ClosestToReactorNoPlayerBetween,InElevatorZone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="H3:H22 Z3:Z22 BK3:BK22 CV3:CV22 EG3:EG22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="H3:H23 Z3:Z23 BK3:BK23 CV3:CV23 EG3:EG23">
       <formula1>"Zone_0,Zone_1,Zone_2,Zone_3,Zone_4,Zone_5,Zone_6,Zone_7,Zone_8,Zone_9,Zone_10,Zone_11,Zone_12,Zone_13,Zone_14,Zone_15,Zone_16,Zone_17,Zone_18,Zone_19,Zone_20"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -4294967296 and 4294967295" sqref="J3:J22 M3:M22 Q3:Q22 S3:S22 AN3:AN22 AV3:AV22 BD3:BD22 BY3:BY22 CG3:CG22 CO3:CO22 DJ3:DJ22 DR3:DR22 DZ3:DZ22 EU3:EU22 FC3:FC22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -4294967296 and 4294967295" sqref="J3:J23 M3:M23 Q3:Q23 S3:S23 AN3:AN23 AV3:AV23 BD3:BD23 BY3:BY23 CG3:CG23 CO3:CO23 DJ3:DJ23 DR3:DR23 DZ3:DZ23 EU3:EU23 FC3:FC23">
       <formula1>-4.294967296E9</formula1>
       <formula2>4.294967295E9</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AI3:AI22 BT3:BT22 DE3:DE22 EP3:EP22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Suggested placeholders." sqref="AI3:AI23 BT3:BT23 DE3:DE23 EP3:EP23">
       <formula1>"low_health_limit,low_health_talk,low_health_grunt,found_health_station_response,oxygen_50,oxygen_25,oxygen_10,oxygen_death,after_damage_fall,on_pick_up_ammo,on_pick_up_health,picked_up_ammo_depleted,on_pick_up_health_when_low,picked_up_keycard_red_a,picke"&amp;"d_up_keycard_blue_a,picked_up_keycard_green_a,picked_up_keycard_yellow_a,picked_up_keycard_white_a,picked_up_keycard_grey_a,picked_up_keycard_black_a,picked_up_keycard_orange_a,picked_up_keycard_purple_a,picked_up_keycard_beige_a,picked_up_keycard_red_b,p"&amp;"icked_up_keycard_blue_b,picked_up_keycard_green_b,picked_up_keycard_yellow_b,picked_up_keycard_white_b,picked_up_keycard_grey_b,picked_up_keycard_black_b,picked_up_keycard_orange_b,picked_up_keycard_purple_b,picked_up_keycard_beige_b,on_ammo_low,ammo_depl"&amp;"eted_reminder,on_reload_weapon_was_out,consumable_depleted_generic,hacking_wrong_first,hacking_wrong_second,hacking_wrong_third,hacking_correct_first,hacking_correct_second,hacking_successful_problematic,hacking_successful_regular,hacking_successful_flawl"&amp;"ess,on_scan_no_enemies,on_scan_few_enemies,on_scan_many_enemies,motion_detector_tagged_plural,on_mapping_finished,cut_lock_first,cut_lock_final,heal_spray_apply_teammate,heal_spray_apply_enemy,sentry_gun_deploy,group_is_not_together,random_comment_pure_st"&amp;"ealth,random_comment_combat_potential,warn_about_tentacles,dark_area_enter,dark_area_light_on,big_space_enter,found_security_post,found_health_station,found_armory,found_scav,found_strongbox,found_resource_box,found_resource_locker,found_meds,found_meds_l"&amp;"ittle,found_ammo,found_ammo_little,idle_no_progress,on_start_open_door,need_keycard_red,need_keycard_blue,need_keycard_green,need_keycard_yellow,need_keycard_white,need_keycard_grey,need_keycard_black,need_keycard_orange,need_keycard_purple,need_keycard_b"&amp;"rown,suggest_keycard_red,suggest_keycard_blue,suggest_keycard_green,suggest_keycard_yellow,suggest_keycard_white,suggest_keycard_grey,suggest_keycard_black,suggest_keycard_orange,suggest_keycard_purple,suggest_keycard_brown,found_node_door,try_to_open_nod"&amp;"e_door,security_door_check,apex_door_to_checkpoint_spot,apex_door_to_elevator_spot,apex_door_fight_anticipation,monster_wave_coming_already_fighting,bio_scan_found,bio_scan_enter,bio_scan_working,generic_done,bio_scan_follow_holo_path,generic_move_to_the_"&amp;"next_one,order_to_bio_scan_woods,order_back_to_bio_scan_woods,order_to_bio_scan_dauda,order_back_to_bio_scan_dauda,order_to_bio_scan_hackett,order_back_to_bio_scan_hackett,order_to_bio_scan_bishop,order_back_to_bio_scan_bishop,accidental_discharge,glottal"&amp;"_stop,caught_by_ceiling_tentacle,land_hard_on_back,shot_yourself_free_from_snatcher,get_shot_free_from_ceiling_tentacle,shoot_parasite_nest,get_parasite,get_parasite_removed,get_parasite_removed_not_all,get_parasite_removed_last,bit_by_parasite,parasite_r"&amp;"emoved_on_teammate,parasite_remove_on_teammate,spot_idle_guard_group,spot_scout,monster_light_sensitivity,killed_single_monster,took_out_scout,attracted_monsters_accident,hear_hunter_group,attracted_monsters_intentional,combat_start,after_damage_generic,a"&amp;"mmo_depleted_taking_damage,man_down_generic,on_char_G_is_downed,on_char_T_is_downed,on_char_F_is_downed,on_char_O_is_downed,help_teammate_up,idle_combat,on_enemy_kill,monsters_breaking_door,monsters_broke_door,friendly_fire_outburst,encounter_over_good,en"&amp;"counter_over_average,encounter_over_bad,encounter_over_scout,on_grabbed_by_tank,held_by_tank,downed_need_help,idle_low_health,death_scream,expedition_start_generic,expedition_start_datamining,expedition_start_scavenge,found_generic_item_1_of_5,found_gener"&amp;"ic_item_2_of_5,found_generic_item_3_of_5,found_generic_item_4_of_5,found_generic_item_final,found_the_item,found_encryption_key_1_of_5,found_encryption_key_2_of_5,found_encryption_key_3_of_5,found_encryption_key_4_of_5,found_encryption_key_final,decon_uni"&amp;"t_briefing,decon_unit_about_to_grab,decon_unit_grabbed,decon_unit_stay_close_reminder,decon_unit_left_behind,get_to_elevator_with_thing,get_to_elevator,get_to_checkpoint_with_thing,get_to_checkpoint,datamining_find_terminal,datamining_found_terminal,datam"&amp;"ining_done_go_to_exit,see_way_to_objective,waypoint_to_data_bank_activated,waypoint_to_checkpoint_activated,waypoint_to_elevator_activated,sneeze,cough_soft,cough_hard,idle_group_bonding,idle_surroundings,just_before_elevator_drop,react_to_woods_log_1,rea"&amp;"ct_to_woods_log_2,react_to_dauda_log_1,react_to_dauda_log_2,react_to_hackett_log_1,react_to_hackett_log_2,react_to_bishop_log_1,react_to_bishop_log_2,ask_for_objective_reminder,find_scav_0,find_scav_1-49,find_scav_50,find_scav_80-99,find_scav_51-79,find_s"&amp;"cav_100,shot_yourself_free_from_ceiling_tentacle,found_item_generic,found_item_succeeding,found_encryption_key_generic,found_encryption_key_succeeding,r06_BigWalkComment,r06_PickUpMWP,r06_TeleportedBackFirstTime,r06_SpotFlyingMonstersFirstTime,r06_Telepor"&amp;"tedMonstersBack,r06_TeleportedFirstTime,CL-Hurry,CL-GoSlow,CL-StandStill,CL-Wait,CL-StayBack,CL-OnMe,CL-North,CL-South,CL-East,CL-West,CL-Left,CL-Right,CL-Middle,CL-FarLeft,CL-FarRight,CL-CheckTheMap,CL-GoQuiet,CL-Shh,CL-WeNeedToPrepare,CL-Synchronize,CL-"&amp;"AreYouReady,CL-ThreeTwoOneGo,CL-GoLoud,CL-BackUp,CL-Scan,CL-WeNeedResources,CL-FocusOnTheObjective,CL-INeedHelp,CL-AlmostThere,CL-Opening,CL-Closing,CL-INeedHealth,CL-MedPackHere,CL-INeedAmmo,CL-AmmoHere,CL-INeedToolRefill,CL-ToolRefillHere,CL-INeedDisinf"&amp;"ection,CL-DisinfectionHere,CL-ResourcesHere,CL-Yes,CL-No,CL-IAgree,CL-IDisagree,CL-Sorry,CL-LetsNotDoThatAgain,CL-WellDone,CL-LotsOfMonstersHere,CL-BigGuyHere,CL-Scout,CL-WeNeedToDoThisTogether,CL-LookUp,CL-RoomClear,CL-Flashlights,CL-IUnderstand,CL-Pleas"&amp;"eRepeatThat,CL-IWillDoIt,CL-NotMe,CL-GrabTheItem,CL-ThisDoor,CL-Terminal,CL-WeNeedATerminal,CL-CFoamHere,CL-TagThem,CL-PutATripmineHere,CL-PutASentryGunHere,CL-ParticleScanHere,CL-WeldThis,CL-NanoSwarmThis,CL-NanoSwarmMe,CL-UseTheNanoSwarm,CL-PickThisUp,C"&amp;"L-ICanDoItShouldI,CL-PickUpYourDeployables,CL-SecureThisRoom,CL-IGotAmmoSomeoneElseCarryThis,CL-Attack,CL-Defend,CL-Please,CL-ThankYou,CL-ImOnMyWay,CL-BRB,CL-CancelThat,CL-Nice,CL-IllTake,CL-YouTake,CL-WeTake,CL-TheOneRightInFrontOfMe,CL-TheOneOnTheRight,"&amp;"CL-TheOneOnTheLeft,CL-TheOneInTheMiddle,CL-TheOneOnTheFarRight,CL-TheOneOnTheFarLeft,CL-TheOneClosestToMe,CL-TheOneClosestToYou,CL-ThisGroup,CL-PickOneEach,CL-LimitedVision,CL-ImExhausted,CL-You,CL-Everyone,CL-Anyone,CL-FollowMe,CL-LetsGTFO,CL-PickUpTheOb"&amp;"jectiveItem,CL-ThrowSomeGlowSticksHere,CL-PutAFogRepellerHere,CL-ICantDoThat,CL-ICantPlaceItThere,CL-IllStayCloseToYou,CL-IllFollowYourLead,CL-ThereAreGlowSticksHere,CL-ThereIsALongRangeFlashlightHere,CL-ThereIsAFogRepellerHere,CL-ThereIsALockMelterHere,C"&amp;"L-ThereIsATripMineHere,CL-ThereIsAFoamMineHere,CL-ThereIsAFoamGrenadeHere,CL-ThereIsARedSyringeHere,CL-ThereIsAYellowSyringeHere,CL-WillDo"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="R3:R22 BC3:BC22 CN3:CN22 DY3:DY22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="R3:R23 BC3:BC23 CN3:CN23 DY3:DY23">
       <formula1>"None,OpenSecurityDoor,UnlockSecurityDoor,AllLightsOff,AllLightsOn,PlaySound,SetFogSetting,DimensionFlashTeam,DimensionWarpTeam,SpawnEnemyWave,StopEnemyWaves,UpdateCustomSubObjective,ForceCompleteObjective,LightsInZone,LightsInZoneToggle,AnimationTrigger,S"&amp;"pawnEnemyOnPoint,SetNavMarker,StepProgressionObjective,SetWorldEventCondition,LockSecurityDoor,SetTerminalCommand,ActivateChainedPuzzle,EventBreak"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="Y3:Y22 BJ3:BJ22 CU3:CU22 EF3:EF22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="Y3:Y23 BJ3:BJ23 CU3:CU23 EF3:EF23">
       <formula1>"Reality,Dimension_1,Dimension_2,Dimension_3,Dimension_4,Dimension_5,Dimension_6,Dimension_7,Dimension_8,Dimension_9,Dimension_10,Dimension_11,Dimension_12,Dimension_13,Dimension_14,Dimension_15,Dimension_16,Dimension_17,Dimension_18,Dimension_19,Dimension"&amp;"_20,MAX_COUNT,ARENA_DIMENSION"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AX3:AX22 CI3:CI22 DT3:DT22 FE3:FE22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Click and enter a value from the list of items" sqref="AX3:AX23 CI3:CI23 DT3:DT23 FE3:FE23">
       <formula1>"None,Help,Commands,Cls,Exit,Open,Close,Activate,Deactivate,EmptyLine,InvalidCommand,DownloadData,ViewSecurityLog,Override,DisableAlarm,Locate,ActivateBeacon,Find,ShowList,Query,Ping,ReactorStartup,ReactorVerify,ReactorShutdown,WardenObjectiveSpecialComman"&amp;"d,TerminalUplinkConnect,TerminalUplinkVerify,TerminalUplinkConfirm,ListLogs,ReadLog,Start,TryUnlockingTerminal,WardenObjectiveGatherCommand,TerminalCorruptedUplinkConnect,TerminalCorruptedUplinkVerify,TimedConnectionSend,TimedConnectionVerify,UsedCommand,"&amp;"UniqueCommand1,UniqueCommand2,UniqueCommand3,UniqueCommand4,UniqueCommand5,Info,MAX_COUNT"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="B3:F22 N3:N22 AA3:AB22 AK3:AK22 AO3:AO22 AS3:AU22 BL3:BM22 BV3:BV22 BZ3:BZ22 CD3:CF22 CW3:CX22 DG3:DG22 DK3:DK22 DO3:DQ22 EH3:EI22 ER3:ER22 EV3:EV22 EZ3:FB22">
+    <dataValidation type="decimal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a number between -3.402823E+38 and 3.402823E+38" sqref="B3:F23 N3:N23 AA3:AB23 AK3:AK23 AO3:AO23 AS3:AU23 BL3:BM23 BV3:BV23 BZ3:BZ23 CD3:CF23 CW3:CX23 DG3:DG23 DK3:DK23 DO3:DQ23 EH3:EI23 ER3:ER23 EV3:EV23 EZ3:FB23">
       <formula1>-3.402823E38</formula1>
       <formula2>3.402823E38</formula2>
     </dataValidation>

</xml_diff>